<commit_message>
UPDATE some db & schedule list
</commit_message>
<xml_diff>
--- a/02.DesignDocument/Project_Management.xlsx
+++ b/02.DesignDocument/Project_Management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\yadanar_thike\02.DesignDocument\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05F717E-79D4-47DB-A1AD-ECE6808FDB4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{582BAE2E-C6A9-42EA-8C22-9AAE913D83DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="3" r:id="rId1"/>
@@ -23,7 +23,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Cover!$A$1:$N$51</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Customer Requirement'!$A$1:$Q$70</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="5">'DB Design'!$A$1:$O$285</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">'DB Design'!$A$1:$O$311</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Schedule!$A$1:$O$93</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1477" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1586" uniqueCount="336">
   <si>
     <t>No</t>
   </si>
@@ -1015,6 +1015,48 @@
   </si>
   <si>
     <t>Admim</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>shop's icon</t>
+  </si>
+  <si>
+    <t>facebook</t>
+  </si>
+  <si>
+    <t>instagram</t>
+  </si>
+  <si>
+    <t>twitter</t>
+  </si>
+  <si>
+    <t>shop's facebook</t>
+  </si>
+  <si>
+    <t>shop's instagram</t>
+  </si>
+  <si>
+    <t>shop's twitter</t>
+  </si>
+  <si>
+    <t>shop list</t>
+  </si>
+  <si>
+    <t>shop's categories</t>
+  </si>
+  <si>
+    <t>phone no.</t>
+  </si>
+  <si>
+    <t>shop's phone</t>
+  </si>
+  <si>
+    <t>shop_Cate</t>
+  </si>
+  <si>
+    <t>shop_name</t>
   </si>
 </sst>
 </file>
@@ -1908,7 +1950,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="574">
+  <cellXfs count="575">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2787,6 +2829,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="11" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2891,12 +2939,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="11" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="53" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
@@ -10192,7 +10237,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A28" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A31" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10489,22 +10534,22 @@
       <c r="N18" s="14"/>
     </row>
     <row r="19" spans="1:14" ht="92.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="537" t="s">
+      <c r="A19" s="543" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="538"/>
-      <c r="C19" s="538"/>
-      <c r="D19" s="538"/>
-      <c r="E19" s="538"/>
-      <c r="F19" s="538"/>
-      <c r="G19" s="538"/>
-      <c r="H19" s="538"/>
-      <c r="I19" s="538"/>
-      <c r="J19" s="538"/>
-      <c r="K19" s="538"/>
-      <c r="L19" s="538"/>
-      <c r="M19" s="538"/>
-      <c r="N19" s="539"/>
+      <c r="B19" s="544"/>
+      <c r="C19" s="544"/>
+      <c r="D19" s="544"/>
+      <c r="E19" s="544"/>
+      <c r="F19" s="544"/>
+      <c r="G19" s="544"/>
+      <c r="H19" s="544"/>
+      <c r="I19" s="544"/>
+      <c r="J19" s="544"/>
+      <c r="K19" s="544"/>
+      <c r="L19" s="544"/>
+      <c r="M19" s="544"/>
+      <c r="N19" s="545"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
@@ -10539,22 +10584,22 @@
       <c r="N21" s="14"/>
     </row>
     <row r="22" spans="1:14" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="A22" s="534" t="s">
+      <c r="A22" s="540" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="535"/>
-      <c r="C22" s="535"/>
-      <c r="D22" s="535"/>
-      <c r="E22" s="535"/>
-      <c r="F22" s="535"/>
-      <c r="G22" s="535"/>
-      <c r="H22" s="535"/>
-      <c r="I22" s="535"/>
-      <c r="J22" s="535"/>
-      <c r="K22" s="535"/>
-      <c r="L22" s="535"/>
-      <c r="M22" s="535"/>
-      <c r="N22" s="536"/>
+      <c r="B22" s="541"/>
+      <c r="C22" s="541"/>
+      <c r="D22" s="541"/>
+      <c r="E22" s="541"/>
+      <c r="F22" s="541"/>
+      <c r="G22" s="541"/>
+      <c r="H22" s="541"/>
+      <c r="I22" s="541"/>
+      <c r="J22" s="541"/>
+      <c r="K22" s="541"/>
+      <c r="L22" s="541"/>
+      <c r="M22" s="541"/>
+      <c r="N22" s="542"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
@@ -10862,10 +10907,10 @@
     </row>
     <row r="42" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A42" s="13"/>
-      <c r="B42" s="532" t="s">
+      <c r="B42" s="538" t="s">
         <v>19</v>
       </c>
-      <c r="C42" s="532"/>
+      <c r="C42" s="538"/>
       <c r="D42" s="20">
         <v>1</v>
       </c>
@@ -10989,13 +11034,13 @@
       <c r="H48" s="6"/>
       <c r="I48" s="6"/>
       <c r="J48" s="6"/>
-      <c r="K48" s="533" t="s">
+      <c r="K48" s="539" t="s">
         <v>21</v>
       </c>
-      <c r="L48" s="533"/>
+      <c r="L48" s="539"/>
       <c r="M48" s="19">
         <f ca="1">NOW()</f>
-        <v>44703.063063541667</v>
+        <v>44703.41012083333</v>
       </c>
       <c r="N48" s="14"/>
     </row>
@@ -11010,13 +11055,13 @@
       <c r="H49" s="6"/>
       <c r="I49" s="6"/>
       <c r="J49" s="6"/>
-      <c r="K49" s="533" t="s">
+      <c r="K49" s="539" t="s">
         <v>20</v>
       </c>
-      <c r="L49" s="533"/>
+      <c r="L49" s="539"/>
       <c r="M49" s="19">
         <f ca="1">NOW()</f>
-        <v>44703.063063541667</v>
+        <v>44703.41012083333</v>
       </c>
       <c r="N49" s="14"/>
     </row>
@@ -11079,54 +11124,54 @@
   <sheetData>
     <row r="1" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:17" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="540" t="s">
+      <c r="A2" s="546" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="541"/>
-      <c r="C2" s="544" t="s">
+      <c r="B2" s="547"/>
+      <c r="C2" s="550" t="s">
         <v>119</v>
       </c>
-      <c r="D2" s="545"/>
-      <c r="E2" s="545"/>
-      <c r="F2" s="545"/>
-      <c r="G2" s="545"/>
-      <c r="H2" s="545"/>
-      <c r="I2" s="545"/>
-      <c r="J2" s="545"/>
-      <c r="K2" s="545"/>
-      <c r="L2" s="545"/>
-      <c r="M2" s="545"/>
-      <c r="N2" s="545"/>
+      <c r="D2" s="551"/>
+      <c r="E2" s="551"/>
+      <c r="F2" s="551"/>
+      <c r="G2" s="551"/>
+      <c r="H2" s="551"/>
+      <c r="I2" s="551"/>
+      <c r="J2" s="551"/>
+      <c r="K2" s="551"/>
+      <c r="L2" s="551"/>
+      <c r="M2" s="551"/>
+      <c r="N2" s="551"/>
       <c r="O2" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="P2" s="548">
+      <c r="P2" s="554">
         <v>44698</v>
       </c>
-      <c r="Q2" s="549"/>
+      <c r="Q2" s="555"/>
     </row>
     <row r="3" spans="1:17" ht="33.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="542"/>
-      <c r="B3" s="543"/>
-      <c r="C3" s="546"/>
-      <c r="D3" s="547"/>
-      <c r="E3" s="547"/>
-      <c r="F3" s="547"/>
-      <c r="G3" s="547"/>
-      <c r="H3" s="547"/>
-      <c r="I3" s="547"/>
-      <c r="J3" s="547"/>
-      <c r="K3" s="547"/>
-      <c r="L3" s="547"/>
-      <c r="M3" s="547"/>
-      <c r="N3" s="547"/>
+      <c r="A3" s="548"/>
+      <c r="B3" s="549"/>
+      <c r="C3" s="552"/>
+      <c r="D3" s="553"/>
+      <c r="E3" s="553"/>
+      <c r="F3" s="553"/>
+      <c r="G3" s="553"/>
+      <c r="H3" s="553"/>
+      <c r="I3" s="553"/>
+      <c r="J3" s="553"/>
+      <c r="K3" s="553"/>
+      <c r="L3" s="553"/>
+      <c r="M3" s="553"/>
+      <c r="N3" s="553"/>
       <c r="O3" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="550">
+      <c r="P3" s="556">
         <v>44698</v>
       </c>
-      <c r="Q3" s="551"/>
+      <c r="Q3" s="557"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
@@ -12168,7 +12213,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O101"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="55" zoomScaleNormal="140" zoomScaleSheetLayoutView="55" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="140" zoomScaleSheetLayoutView="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12185,50 +12230,50 @@
   <sheetData>
     <row r="1" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:15" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="540" t="s">
+      <c r="A2" s="546" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="541"/>
-      <c r="C2" s="544" t="s">
+      <c r="B2" s="547"/>
+      <c r="C2" s="550" t="s">
         <v>119</v>
       </c>
-      <c r="D2" s="545"/>
-      <c r="E2" s="545"/>
-      <c r="F2" s="545"/>
-      <c r="G2" s="545"/>
-      <c r="H2" s="545"/>
-      <c r="I2" s="545"/>
-      <c r="J2" s="545"/>
-      <c r="K2" s="545"/>
-      <c r="L2" s="545"/>
+      <c r="D2" s="551"/>
+      <c r="E2" s="551"/>
+      <c r="F2" s="551"/>
+      <c r="G2" s="551"/>
+      <c r="H2" s="551"/>
+      <c r="I2" s="551"/>
+      <c r="J2" s="551"/>
+      <c r="K2" s="551"/>
+      <c r="L2" s="551"/>
       <c r="M2" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="548">
+      <c r="N2" s="554">
         <v>44698</v>
       </c>
-      <c r="O2" s="549"/>
+      <c r="O2" s="555"/>
     </row>
     <row r="3" spans="1:15" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="542"/>
-      <c r="B3" s="543"/>
-      <c r="C3" s="546"/>
-      <c r="D3" s="547"/>
-      <c r="E3" s="547"/>
-      <c r="F3" s="547"/>
-      <c r="G3" s="547"/>
-      <c r="H3" s="547"/>
-      <c r="I3" s="547"/>
-      <c r="J3" s="547"/>
-      <c r="K3" s="547"/>
-      <c r="L3" s="547"/>
+      <c r="A3" s="548"/>
+      <c r="B3" s="549"/>
+      <c r="C3" s="552"/>
+      <c r="D3" s="553"/>
+      <c r="E3" s="553"/>
+      <c r="F3" s="553"/>
+      <c r="G3" s="553"/>
+      <c r="H3" s="553"/>
+      <c r="I3" s="553"/>
+      <c r="J3" s="553"/>
+      <c r="K3" s="553"/>
+      <c r="L3" s="553"/>
       <c r="M3" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="N3" s="550">
+      <c r="N3" s="556">
         <v>44698</v>
       </c>
-      <c r="O3" s="551"/>
+      <c r="O3" s="557"/>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
@@ -12417,7 +12462,7 @@
       <c r="I10" s="82">
         <v>44699</v>
       </c>
-      <c r="J10" s="571">
+      <c r="J10" s="535">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -12452,7 +12497,7 @@
       <c r="I11" s="82">
         <v>44699</v>
       </c>
-      <c r="J11" s="571">
+      <c r="J11" s="535">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -12487,7 +12532,7 @@
       <c r="I12" s="82">
         <v>44699</v>
       </c>
-      <c r="J12" s="571">
+      <c r="J12" s="535">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -12522,7 +12567,7 @@
       <c r="I13" s="87">
         <v>44699</v>
       </c>
-      <c r="J13" s="572">
+      <c r="J13" s="536">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -12557,7 +12602,7 @@
       <c r="I14" s="82">
         <v>44699</v>
       </c>
-      <c r="J14" s="571">
+      <c r="J14" s="535">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -12592,7 +12637,7 @@
       <c r="I15" s="87">
         <v>44699</v>
       </c>
-      <c r="J15" s="572">
+      <c r="J15" s="536">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -12627,7 +12672,7 @@
       <c r="I16" s="82">
         <v>44700</v>
       </c>
-      <c r="J16" s="571">
+      <c r="J16" s="535">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -12662,7 +12707,7 @@
       <c r="I17" s="87">
         <v>44700</v>
       </c>
-      <c r="J17" s="572">
+      <c r="J17" s="536">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -12697,7 +12742,7 @@
       <c r="I18" s="87">
         <v>44700</v>
       </c>
-      <c r="J18" s="572">
+      <c r="J18" s="536">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -12732,7 +12777,7 @@
       <c r="I19" s="87">
         <v>44700</v>
       </c>
-      <c r="J19" s="572">
+      <c r="J19" s="536">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -12767,7 +12812,7 @@
       <c r="I20" s="87">
         <v>44700</v>
       </c>
-      <c r="J20" s="572">
+      <c r="J20" s="536">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -12802,7 +12847,7 @@
       <c r="I21" s="87">
         <v>44700</v>
       </c>
-      <c r="J21" s="572">
+      <c r="J21" s="536">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -12837,7 +12882,7 @@
       <c r="I22" s="87">
         <v>44700</v>
       </c>
-      <c r="J22" s="572">
+      <c r="J22" s="536">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -12872,7 +12917,7 @@
       <c r="I23" s="87">
         <v>44700</v>
       </c>
-      <c r="J23" s="572">
+      <c r="J23" s="536">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -12907,7 +12952,7 @@
       <c r="I24" s="87">
         <v>44700</v>
       </c>
-      <c r="J24" s="572">
+      <c r="J24" s="536">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -12942,7 +12987,7 @@
       <c r="I25" s="87">
         <v>44700</v>
       </c>
-      <c r="J25" s="572">
+      <c r="J25" s="536">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -12977,7 +13022,7 @@
       <c r="I26" s="87">
         <v>44700</v>
       </c>
-      <c r="J26" s="572">
+      <c r="J26" s="536">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -13012,7 +13057,7 @@
       <c r="I27" s="87">
         <v>44700</v>
       </c>
-      <c r="J27" s="572">
+      <c r="J27" s="536">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -13047,7 +13092,7 @@
       <c r="I28" s="87">
         <v>44700</v>
       </c>
-      <c r="J28" s="572">
+      <c r="J28" s="536">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -13082,7 +13127,7 @@
       <c r="I29" s="82">
         <v>44700</v>
       </c>
-      <c r="J29" s="571">
+      <c r="J29" s="535">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -13138,7 +13183,7 @@
       <c r="I31" s="481">
         <v>44699</v>
       </c>
-      <c r="J31" s="569">
+      <c r="J31" s="533">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -13173,7 +13218,7 @@
       <c r="I32" s="481">
         <v>44699</v>
       </c>
-      <c r="J32" s="569">
+      <c r="J32" s="533">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -13208,7 +13253,7 @@
       <c r="I33" s="491">
         <v>44700</v>
       </c>
-      <c r="J33" s="568">
+      <c r="J33" s="532">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -13243,7 +13288,7 @@
       <c r="I34" s="481">
         <v>44700</v>
       </c>
-      <c r="J34" s="569">
+      <c r="J34" s="533">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -13278,7 +13323,7 @@
       <c r="I35" s="491">
         <v>44701</v>
       </c>
-      <c r="J35" s="568">
+      <c r="J35" s="532">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -13313,7 +13358,7 @@
       <c r="I36" s="491">
         <v>44701</v>
       </c>
-      <c r="J36" s="568">
+      <c r="J36" s="532">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -13348,7 +13393,7 @@
       <c r="I37" s="481">
         <v>44700</v>
       </c>
-      <c r="J37" s="569">
+      <c r="J37" s="533">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -13383,7 +13428,7 @@
       <c r="I38" s="481">
         <v>44701</v>
       </c>
-      <c r="J38" s="569">
+      <c r="J38" s="533">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -13418,7 +13463,7 @@
       <c r="I39" s="486">
         <v>44699</v>
       </c>
-      <c r="J39" s="570">
+      <c r="J39" s="534">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -13453,7 +13498,7 @@
       <c r="I40" s="486">
         <v>44700</v>
       </c>
-      <c r="J40" s="570">
+      <c r="J40" s="534">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -13488,7 +13533,7 @@
       <c r="I41" s="486">
         <v>44700</v>
       </c>
-      <c r="J41" s="570">
+      <c r="J41" s="534">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -13523,7 +13568,7 @@
       <c r="I42" s="481">
         <v>44702</v>
       </c>
-      <c r="J42" s="569">
+      <c r="J42" s="533">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
@@ -13558,7 +13603,7 @@
       <c r="I43" s="481">
         <v>44702</v>
       </c>
-      <c r="J43" s="569">
+      <c r="J43" s="533">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
@@ -13593,7 +13638,7 @@
       <c r="I44" s="486">
         <v>44699</v>
       </c>
-      <c r="J44" s="570">
+      <c r="J44" s="534">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -13628,7 +13673,7 @@
       <c r="I45" s="481">
         <v>44701</v>
       </c>
-      <c r="J45" s="569">
+      <c r="J45" s="533">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -13660,12 +13705,16 @@
       <c r="H46" s="491">
         <v>44698</v>
       </c>
-      <c r="I46" s="491"/>
-      <c r="J46" s="568">
+      <c r="I46" s="491">
+        <v>44703</v>
+      </c>
+      <c r="J46" s="532">
         <f t="shared" si="1"/>
-        <v>-44698</v>
-      </c>
-      <c r="K46" s="492"/>
+        <v>5</v>
+      </c>
+      <c r="K46" s="492">
+        <v>0.9</v>
+      </c>
     </row>
     <row r="47" spans="1:11" s="421" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A47" s="478"/>
@@ -14758,68 +14807,68 @@
   <sheetData>
     <row r="1" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:24" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="540" t="s">
+      <c r="A2" s="546" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="541"/>
-      <c r="C2" s="544" t="s">
+      <c r="B2" s="547"/>
+      <c r="C2" s="550" t="s">
         <v>119</v>
       </c>
-      <c r="D2" s="545"/>
-      <c r="E2" s="545"/>
-      <c r="F2" s="545"/>
-      <c r="G2" s="545"/>
-      <c r="H2" s="545"/>
-      <c r="I2" s="545"/>
-      <c r="J2" s="545"/>
-      <c r="K2" s="545"/>
-      <c r="L2" s="545"/>
-      <c r="M2" s="545"/>
-      <c r="N2" s="545"/>
-      <c r="O2" s="545"/>
-      <c r="P2" s="545"/>
-      <c r="Q2" s="545"/>
-      <c r="R2" s="545"/>
-      <c r="S2" s="545"/>
-      <c r="T2" s="545"/>
-      <c r="U2" s="545"/>
+      <c r="D2" s="551"/>
+      <c r="E2" s="551"/>
+      <c r="F2" s="551"/>
+      <c r="G2" s="551"/>
+      <c r="H2" s="551"/>
+      <c r="I2" s="551"/>
+      <c r="J2" s="551"/>
+      <c r="K2" s="551"/>
+      <c r="L2" s="551"/>
+      <c r="M2" s="551"/>
+      <c r="N2" s="551"/>
+      <c r="O2" s="551"/>
+      <c r="P2" s="551"/>
+      <c r="Q2" s="551"/>
+      <c r="R2" s="551"/>
+      <c r="S2" s="551"/>
+      <c r="T2" s="551"/>
+      <c r="U2" s="551"/>
       <c r="V2" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="W2" s="548">
+      <c r="W2" s="554">
         <v>44698</v>
       </c>
-      <c r="X2" s="549"/>
+      <c r="X2" s="555"/>
     </row>
     <row r="3" spans="1:24" ht="33.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="542"/>
-      <c r="B3" s="543"/>
-      <c r="C3" s="546"/>
-      <c r="D3" s="547"/>
-      <c r="E3" s="547"/>
-      <c r="F3" s="547"/>
-      <c r="G3" s="547"/>
-      <c r="H3" s="547"/>
-      <c r="I3" s="547"/>
-      <c r="J3" s="547"/>
-      <c r="K3" s="547"/>
-      <c r="L3" s="547"/>
-      <c r="M3" s="547"/>
-      <c r="N3" s="547"/>
-      <c r="O3" s="547"/>
-      <c r="P3" s="547"/>
-      <c r="Q3" s="547"/>
-      <c r="R3" s="547"/>
-      <c r="S3" s="547"/>
-      <c r="T3" s="547"/>
-      <c r="U3" s="547"/>
+      <c r="A3" s="548"/>
+      <c r="B3" s="549"/>
+      <c r="C3" s="552"/>
+      <c r="D3" s="553"/>
+      <c r="E3" s="553"/>
+      <c r="F3" s="553"/>
+      <c r="G3" s="553"/>
+      <c r="H3" s="553"/>
+      <c r="I3" s="553"/>
+      <c r="J3" s="553"/>
+      <c r="K3" s="553"/>
+      <c r="L3" s="553"/>
+      <c r="M3" s="553"/>
+      <c r="N3" s="553"/>
+      <c r="O3" s="553"/>
+      <c r="P3" s="553"/>
+      <c r="Q3" s="553"/>
+      <c r="R3" s="553"/>
+      <c r="S3" s="553"/>
+      <c r="T3" s="553"/>
+      <c r="U3" s="553"/>
       <c r="V3" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="W3" s="550">
+      <c r="W3" s="556">
         <v>44698</v>
       </c>
-      <c r="X3" s="551"/>
+      <c r="X3" s="557"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
@@ -14853,26 +14902,26 @@
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
-      <c r="D5" s="559"/>
-      <c r="E5" s="560"/>
-      <c r="F5" s="560"/>
-      <c r="G5" s="560"/>
-      <c r="H5" s="560"/>
-      <c r="I5" s="560"/>
-      <c r="J5" s="560"/>
-      <c r="K5" s="560"/>
-      <c r="L5" s="560"/>
-      <c r="M5" s="560"/>
-      <c r="N5" s="560"/>
-      <c r="O5" s="560"/>
-      <c r="P5" s="560"/>
-      <c r="Q5" s="560"/>
-      <c r="R5" s="560"/>
-      <c r="S5" s="560"/>
-      <c r="T5" s="560"/>
-      <c r="U5" s="560"/>
-      <c r="V5" s="560"/>
-      <c r="W5" s="561"/>
+      <c r="D5" s="565"/>
+      <c r="E5" s="566"/>
+      <c r="F5" s="566"/>
+      <c r="G5" s="566"/>
+      <c r="H5" s="566"/>
+      <c r="I5" s="566"/>
+      <c r="J5" s="566"/>
+      <c r="K5" s="566"/>
+      <c r="L5" s="566"/>
+      <c r="M5" s="566"/>
+      <c r="N5" s="566"/>
+      <c r="O5" s="566"/>
+      <c r="P5" s="566"/>
+      <c r="Q5" s="566"/>
+      <c r="R5" s="566"/>
+      <c r="S5" s="566"/>
+      <c r="T5" s="566"/>
+      <c r="U5" s="566"/>
+      <c r="V5" s="566"/>
+      <c r="W5" s="567"/>
       <c r="X5" s="14"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -14881,104 +14930,104 @@
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
-      <c r="D6" s="562"/>
-      <c r="E6" s="563"/>
-      <c r="F6" s="563"/>
-      <c r="G6" s="563"/>
-      <c r="H6" s="563"/>
-      <c r="I6" s="563"/>
-      <c r="J6" s="563"/>
-      <c r="K6" s="563"/>
-      <c r="L6" s="563"/>
-      <c r="M6" s="563"/>
-      <c r="N6" s="563"/>
-      <c r="O6" s="563"/>
-      <c r="P6" s="563"/>
-      <c r="Q6" s="563"/>
-      <c r="R6" s="563"/>
-      <c r="S6" s="563"/>
-      <c r="T6" s="563"/>
-      <c r="U6" s="563"/>
-      <c r="V6" s="563"/>
-      <c r="W6" s="564"/>
+      <c r="D6" s="568"/>
+      <c r="E6" s="569"/>
+      <c r="F6" s="569"/>
+      <c r="G6" s="569"/>
+      <c r="H6" s="569"/>
+      <c r="I6" s="569"/>
+      <c r="J6" s="569"/>
+      <c r="K6" s="569"/>
+      <c r="L6" s="569"/>
+      <c r="M6" s="569"/>
+      <c r="N6" s="569"/>
+      <c r="O6" s="569"/>
+      <c r="P6" s="569"/>
+      <c r="Q6" s="569"/>
+      <c r="R6" s="569"/>
+      <c r="S6" s="569"/>
+      <c r="T6" s="569"/>
+      <c r="U6" s="569"/>
+      <c r="V6" s="569"/>
+      <c r="W6" s="570"/>
       <c r="X6" s="14"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
-      <c r="D7" s="562"/>
-      <c r="E7" s="563"/>
-      <c r="F7" s="563"/>
-      <c r="G7" s="563"/>
-      <c r="H7" s="563"/>
-      <c r="I7" s="563"/>
-      <c r="J7" s="563"/>
-      <c r="K7" s="563"/>
-      <c r="L7" s="563"/>
-      <c r="M7" s="563"/>
-      <c r="N7" s="563"/>
-      <c r="O7" s="563"/>
-      <c r="P7" s="563"/>
-      <c r="Q7" s="563"/>
-      <c r="R7" s="563"/>
-      <c r="S7" s="563"/>
-      <c r="T7" s="563"/>
-      <c r="U7" s="563"/>
-      <c r="V7" s="563"/>
-      <c r="W7" s="564"/>
+      <c r="D7" s="568"/>
+      <c r="E7" s="569"/>
+      <c r="F7" s="569"/>
+      <c r="G7" s="569"/>
+      <c r="H7" s="569"/>
+      <c r="I7" s="569"/>
+      <c r="J7" s="569"/>
+      <c r="K7" s="569"/>
+      <c r="L7" s="569"/>
+      <c r="M7" s="569"/>
+      <c r="N7" s="569"/>
+      <c r="O7" s="569"/>
+      <c r="P7" s="569"/>
+      <c r="Q7" s="569"/>
+      <c r="R7" s="569"/>
+      <c r="S7" s="569"/>
+      <c r="T7" s="569"/>
+      <c r="U7" s="569"/>
+      <c r="V7" s="569"/>
+      <c r="W7" s="570"/>
       <c r="X7" s="14"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
-      <c r="D8" s="562"/>
-      <c r="E8" s="563"/>
-      <c r="F8" s="563"/>
-      <c r="G8" s="563"/>
-      <c r="H8" s="563"/>
-      <c r="I8" s="563"/>
-      <c r="J8" s="563"/>
-      <c r="K8" s="563"/>
-      <c r="L8" s="563"/>
-      <c r="M8" s="563"/>
-      <c r="N8" s="563"/>
-      <c r="O8" s="563"/>
-      <c r="P8" s="563"/>
-      <c r="Q8" s="563"/>
-      <c r="R8" s="563"/>
-      <c r="S8" s="563"/>
-      <c r="T8" s="563"/>
-      <c r="U8" s="563"/>
-      <c r="V8" s="563"/>
-      <c r="W8" s="564"/>
+      <c r="D8" s="568"/>
+      <c r="E8" s="569"/>
+      <c r="F8" s="569"/>
+      <c r="G8" s="569"/>
+      <c r="H8" s="569"/>
+      <c r="I8" s="569"/>
+      <c r="J8" s="569"/>
+      <c r="K8" s="569"/>
+      <c r="L8" s="569"/>
+      <c r="M8" s="569"/>
+      <c r="N8" s="569"/>
+      <c r="O8" s="569"/>
+      <c r="P8" s="569"/>
+      <c r="Q8" s="569"/>
+      <c r="R8" s="569"/>
+      <c r="S8" s="569"/>
+      <c r="T8" s="569"/>
+      <c r="U8" s="569"/>
+      <c r="V8" s="569"/>
+      <c r="W8" s="570"/>
       <c r="X8" s="14"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="565"/>
-      <c r="E9" s="566"/>
-      <c r="F9" s="566"/>
-      <c r="G9" s="566"/>
-      <c r="H9" s="566"/>
-      <c r="I9" s="566"/>
-      <c r="J9" s="566"/>
-      <c r="K9" s="566"/>
-      <c r="L9" s="566"/>
-      <c r="M9" s="566"/>
-      <c r="N9" s="566"/>
-      <c r="O9" s="566"/>
-      <c r="P9" s="566"/>
-      <c r="Q9" s="566"/>
-      <c r="R9" s="566"/>
-      <c r="S9" s="566"/>
-      <c r="T9" s="566"/>
-      <c r="U9" s="566"/>
-      <c r="V9" s="566"/>
-      <c r="W9" s="567"/>
+      <c r="D9" s="571"/>
+      <c r="E9" s="572"/>
+      <c r="F9" s="572"/>
+      <c r="G9" s="572"/>
+      <c r="H9" s="572"/>
+      <c r="I9" s="572"/>
+      <c r="J9" s="572"/>
+      <c r="K9" s="572"/>
+      <c r="L9" s="572"/>
+      <c r="M9" s="572"/>
+      <c r="N9" s="572"/>
+      <c r="O9" s="572"/>
+      <c r="P9" s="572"/>
+      <c r="Q9" s="572"/>
+      <c r="R9" s="572"/>
+      <c r="S9" s="572"/>
+      <c r="T9" s="572"/>
+      <c r="U9" s="572"/>
+      <c r="V9" s="572"/>
+      <c r="W9" s="573"/>
       <c r="X9" s="14"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
@@ -15008,58 +15057,58 @@
       <c r="X10" s="14"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="552" t="s">
+      <c r="A11" s="558" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="553"/>
-      <c r="C11" s="553"/>
-      <c r="D11" s="553"/>
-      <c r="E11" s="553"/>
-      <c r="F11" s="553"/>
-      <c r="G11" s="553"/>
-      <c r="H11" s="553"/>
-      <c r="I11" s="553"/>
-      <c r="J11" s="553"/>
-      <c r="K11" s="553"/>
-      <c r="L11" s="553"/>
-      <c r="M11" s="553"/>
-      <c r="N11" s="553"/>
-      <c r="O11" s="553"/>
-      <c r="P11" s="553"/>
-      <c r="Q11" s="553"/>
-      <c r="R11" s="553"/>
-      <c r="S11" s="553"/>
-      <c r="T11" s="553"/>
-      <c r="U11" s="553"/>
-      <c r="V11" s="553"/>
-      <c r="W11" s="553"/>
-      <c r="X11" s="554"/>
+      <c r="B11" s="559"/>
+      <c r="C11" s="559"/>
+      <c r="D11" s="559"/>
+      <c r="E11" s="559"/>
+      <c r="F11" s="559"/>
+      <c r="G11" s="559"/>
+      <c r="H11" s="559"/>
+      <c r="I11" s="559"/>
+      <c r="J11" s="559"/>
+      <c r="K11" s="559"/>
+      <c r="L11" s="559"/>
+      <c r="M11" s="559"/>
+      <c r="N11" s="559"/>
+      <c r="O11" s="559"/>
+      <c r="P11" s="559"/>
+      <c r="Q11" s="559"/>
+      <c r="R11" s="559"/>
+      <c r="S11" s="559"/>
+      <c r="T11" s="559"/>
+      <c r="U11" s="559"/>
+      <c r="V11" s="559"/>
+      <c r="W11" s="559"/>
+      <c r="X11" s="560"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12" s="555"/>
-      <c r="B12" s="556"/>
-      <c r="C12" s="556"/>
-      <c r="D12" s="556"/>
-      <c r="E12" s="556"/>
-      <c r="F12" s="556"/>
-      <c r="G12" s="556"/>
-      <c r="H12" s="556"/>
-      <c r="I12" s="557"/>
-      <c r="J12" s="556"/>
-      <c r="K12" s="556"/>
-      <c r="L12" s="556"/>
-      <c r="M12" s="556"/>
-      <c r="N12" s="556"/>
-      <c r="O12" s="556"/>
-      <c r="P12" s="556"/>
-      <c r="Q12" s="556"/>
-      <c r="R12" s="556"/>
-      <c r="S12" s="556"/>
-      <c r="T12" s="556"/>
-      <c r="U12" s="556"/>
-      <c r="V12" s="556"/>
-      <c r="W12" s="556"/>
-      <c r="X12" s="558"/>
+      <c r="A12" s="561"/>
+      <c r="B12" s="562"/>
+      <c r="C12" s="562"/>
+      <c r="D12" s="562"/>
+      <c r="E12" s="562"/>
+      <c r="F12" s="562"/>
+      <c r="G12" s="562"/>
+      <c r="H12" s="562"/>
+      <c r="I12" s="563"/>
+      <c r="J12" s="562"/>
+      <c r="K12" s="562"/>
+      <c r="L12" s="562"/>
+      <c r="M12" s="562"/>
+      <c r="N12" s="562"/>
+      <c r="O12" s="562"/>
+      <c r="P12" s="562"/>
+      <c r="Q12" s="562"/>
+      <c r="R12" s="562"/>
+      <c r="S12" s="562"/>
+      <c r="T12" s="562"/>
+      <c r="U12" s="562"/>
+      <c r="V12" s="562"/>
+      <c r="W12" s="562"/>
+      <c r="X12" s="564"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="29"/>
@@ -16873,7 +16922,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q72"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A10" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16883,54 +16932,54 @@
   <sheetData>
     <row r="1" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:17" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="540" t="s">
+      <c r="A2" s="546" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="541"/>
-      <c r="C2" s="544" t="s">
+      <c r="B2" s="547"/>
+      <c r="C2" s="550" t="s">
         <v>119</v>
       </c>
-      <c r="D2" s="545"/>
-      <c r="E2" s="545"/>
-      <c r="F2" s="545"/>
-      <c r="G2" s="545"/>
-      <c r="H2" s="545"/>
-      <c r="I2" s="545"/>
-      <c r="J2" s="545"/>
-      <c r="K2" s="545"/>
-      <c r="L2" s="545"/>
-      <c r="M2" s="545"/>
-      <c r="N2" s="545"/>
+      <c r="D2" s="551"/>
+      <c r="E2" s="551"/>
+      <c r="F2" s="551"/>
+      <c r="G2" s="551"/>
+      <c r="H2" s="551"/>
+      <c r="I2" s="551"/>
+      <c r="J2" s="551"/>
+      <c r="K2" s="551"/>
+      <c r="L2" s="551"/>
+      <c r="M2" s="551"/>
+      <c r="N2" s="551"/>
       <c r="O2" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="P2" s="548">
+      <c r="P2" s="554">
         <v>44698</v>
       </c>
-      <c r="Q2" s="549"/>
+      <c r="Q2" s="555"/>
     </row>
     <row r="3" spans="1:17" ht="33.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="542"/>
-      <c r="B3" s="543"/>
-      <c r="C3" s="546"/>
-      <c r="D3" s="547"/>
-      <c r="E3" s="547"/>
-      <c r="F3" s="547"/>
-      <c r="G3" s="547"/>
-      <c r="H3" s="547"/>
-      <c r="I3" s="547"/>
-      <c r="J3" s="547"/>
-      <c r="K3" s="547"/>
-      <c r="L3" s="547"/>
-      <c r="M3" s="547"/>
-      <c r="N3" s="547"/>
+      <c r="A3" s="548"/>
+      <c r="B3" s="549"/>
+      <c r="C3" s="552"/>
+      <c r="D3" s="553"/>
+      <c r="E3" s="553"/>
+      <c r="F3" s="553"/>
+      <c r="G3" s="553"/>
+      <c r="H3" s="553"/>
+      <c r="I3" s="553"/>
+      <c r="J3" s="553"/>
+      <c r="K3" s="553"/>
+      <c r="L3" s="553"/>
+      <c r="M3" s="553"/>
+      <c r="N3" s="553"/>
       <c r="O3" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="550">
+      <c r="P3" s="556">
         <v>44698</v>
       </c>
-      <c r="Q3" s="551"/>
+      <c r="Q3" s="557"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
@@ -18259,9 +18308,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:O279"/>
+  <dimension ref="A1:O301"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="55" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -18276,50 +18325,50 @@
   <sheetData>
     <row r="1" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:15" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="540" t="s">
+      <c r="A2" s="546" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="541"/>
-      <c r="C2" s="544" t="s">
+      <c r="B2" s="547"/>
+      <c r="C2" s="550" t="s">
         <v>119</v>
       </c>
-      <c r="D2" s="545"/>
-      <c r="E2" s="545"/>
-      <c r="F2" s="545"/>
-      <c r="G2" s="545"/>
-      <c r="H2" s="545"/>
-      <c r="I2" s="545"/>
-      <c r="J2" s="545"/>
-      <c r="K2" s="545"/>
-      <c r="L2" s="545"/>
+      <c r="D2" s="551"/>
+      <c r="E2" s="551"/>
+      <c r="F2" s="551"/>
+      <c r="G2" s="551"/>
+      <c r="H2" s="551"/>
+      <c r="I2" s="551"/>
+      <c r="J2" s="551"/>
+      <c r="K2" s="551"/>
+      <c r="L2" s="551"/>
       <c r="M2" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="548">
+      <c r="N2" s="554">
         <v>44698</v>
       </c>
-      <c r="O2" s="549"/>
+      <c r="O2" s="555"/>
     </row>
     <row r="3" spans="1:15" ht="33.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="542"/>
-      <c r="B3" s="543"/>
-      <c r="C3" s="546"/>
-      <c r="D3" s="547"/>
-      <c r="E3" s="547"/>
-      <c r="F3" s="547"/>
-      <c r="G3" s="547"/>
-      <c r="H3" s="547"/>
-      <c r="I3" s="547"/>
-      <c r="J3" s="547"/>
-      <c r="K3" s="547"/>
-      <c r="L3" s="547"/>
+      <c r="A3" s="548"/>
+      <c r="B3" s="549"/>
+      <c r="C3" s="552"/>
+      <c r="D3" s="553"/>
+      <c r="E3" s="553"/>
+      <c r="F3" s="553"/>
+      <c r="G3" s="553"/>
+      <c r="H3" s="553"/>
+      <c r="I3" s="553"/>
+      <c r="J3" s="553"/>
+      <c r="K3" s="553"/>
+      <c r="L3" s="553"/>
       <c r="M3" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="N3" s="550">
+      <c r="N3" s="556">
         <v>44702</v>
       </c>
-      <c r="O3" s="551"/>
+      <c r="O3" s="557"/>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13"/>
@@ -20168,10 +20217,10 @@
         <v>145</v>
       </c>
       <c r="H66" s="328" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I66" s="327">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J66" s="327"/>
       <c r="K66" s="329"/>
@@ -20710,10 +20759,10 @@
         <v>145</v>
       </c>
       <c r="H84" s="373" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I84" s="372">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J84" s="372"/>
       <c r="K84" s="374"/>
@@ -21354,10 +21403,10 @@
         <v>145</v>
       </c>
       <c r="H108" s="412" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I108" s="411">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J108" s="411"/>
       <c r="K108" s="413"/>
@@ -22028,10 +22077,10 @@
         <v>145</v>
       </c>
       <c r="H130" s="458" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I130" s="457">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J130" s="457"/>
       <c r="K130" s="459"/>
@@ -22403,10 +22452,10 @@
         <v>145</v>
       </c>
       <c r="H143" s="458" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I143" s="457">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J143" s="457"/>
       <c r="K143" s="459"/>
@@ -22955,7 +23004,7 @@
       <c r="N161" s="494"/>
       <c r="O161" s="495"/>
     </row>
-    <row r="162" spans="1:15" s="573" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:15" s="537" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A162" s="465"/>
       <c r="B162" s="470"/>
       <c r="C162" s="470"/>
@@ -22972,7 +23021,7 @@
       <c r="N162" s="470"/>
       <c r="O162" s="471"/>
     </row>
-    <row r="163" spans="1:15" s="573" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:15" s="537" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="465"/>
       <c r="L163" s="470"/>
       <c r="M163" s="470"/>
@@ -23266,10 +23315,10 @@
         <v>145</v>
       </c>
       <c r="H173" s="117" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I173" s="116">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J173" s="116"/>
       <c r="K173" s="118"/>
@@ -23677,10 +23726,10 @@
         <v>145</v>
       </c>
       <c r="H200" s="160" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I200" s="159">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J200" s="159"/>
       <c r="K200" s="161"/>
@@ -24120,10 +24169,10 @@
         <v>145</v>
       </c>
       <c r="H215" s="160" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I215" s="159">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J215" s="159"/>
       <c r="K215" s="161"/>
@@ -24492,10 +24541,10 @@
         <v>145</v>
       </c>
       <c r="H229" s="458" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I229" s="457">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J229" s="457"/>
       <c r="K229" s="459"/>
@@ -24841,10 +24890,10 @@
         <v>145</v>
       </c>
       <c r="H243" s="458" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I243" s="457">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J243" s="457"/>
       <c r="K243" s="459"/>
@@ -25221,10 +25270,10 @@
         <v>145</v>
       </c>
       <c r="H258" s="458" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I258" s="457">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J258" s="457"/>
       <c r="K258" s="459"/>
@@ -25493,10 +25542,10 @@
         <v>4</v>
       </c>
       <c r="C270" s="462" t="s">
-        <v>309</v>
+        <v>322</v>
       </c>
       <c r="D270" s="462" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="E270" s="430" t="s">
         <v>146</v>
@@ -25508,10 +25557,10 @@
         <v>145</v>
       </c>
       <c r="H270" s="462" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I270" s="472">
-        <v>11</v>
+        <v>256</v>
       </c>
       <c r="J270" s="463"/>
       <c r="K270" s="477"/>
@@ -25526,10 +25575,10 @@
         <v>5</v>
       </c>
       <c r="C271" s="462" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D271" s="462" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="E271" s="430" t="s">
         <v>146</v>
@@ -25544,7 +25593,7 @@
         <v>148</v>
       </c>
       <c r="I271" s="472">
-        <v>256</v>
+        <v>20</v>
       </c>
       <c r="J271" s="463"/>
       <c r="K271" s="477"/>
@@ -25559,10 +25608,10 @@
         <v>6</v>
       </c>
       <c r="C272" s="462" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D272" s="462" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E272" s="430" t="s">
         <v>146</v>
@@ -25592,10 +25641,10 @@
         <v>7</v>
       </c>
       <c r="C273" s="462" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D273" s="462" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E273" s="430" t="s">
         <v>146</v>
@@ -25625,10 +25674,10 @@
         <v>8</v>
       </c>
       <c r="C274" s="462" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D274" s="462" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E274" s="430" t="s">
         <v>146</v>
@@ -25657,64 +25706,62 @@
       <c r="B275" s="428">
         <v>9</v>
       </c>
-      <c r="C275" s="429" t="s">
-        <v>166</v>
-      </c>
-      <c r="D275" s="429" t="s">
-        <v>167</v>
+      <c r="C275" s="462" t="s">
+        <v>313</v>
+      </c>
+      <c r="D275" s="462" t="s">
+        <v>320</v>
       </c>
       <c r="E275" s="430" t="s">
         <v>146</v>
       </c>
-      <c r="F275" s="430" t="s">
+      <c r="F275" s="472" t="s">
         <v>146</v>
       </c>
       <c r="G275" s="430" t="s">
         <v>145</v>
       </c>
-      <c r="H275" s="431" t="s">
-        <v>147</v>
-      </c>
-      <c r="I275" s="430">
-        <v>11</v>
-      </c>
-      <c r="J275" s="430"/>
-      <c r="K275" s="288" t="s">
-        <v>168</v>
-      </c>
+      <c r="H275" s="462" t="s">
+        <v>148</v>
+      </c>
+      <c r="I275" s="472">
+        <v>256</v>
+      </c>
+      <c r="J275" s="463"/>
+      <c r="K275" s="477"/>
       <c r="L275" s="422"/>
       <c r="M275" s="422"/>
       <c r="N275" s="422"/>
       <c r="O275" s="424"/>
     </row>
     <row r="276" spans="1:15" s="421" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A276" s="465"/>
+      <c r="A276" s="423"/>
       <c r="B276" s="428">
         <v>10</v>
       </c>
-      <c r="C276" s="456" t="s">
-        <v>154</v>
-      </c>
-      <c r="D276" s="456" t="s">
-        <v>159</v>
+      <c r="C276" s="462" t="s">
+        <v>324</v>
+      </c>
+      <c r="D276" s="462" t="s">
+        <v>327</v>
       </c>
       <c r="E276" s="430" t="s">
         <v>146</v>
       </c>
-      <c r="F276" s="430" t="s">
-        <v>146</v>
-      </c>
-      <c r="G276" s="457" t="s">
+      <c r="F276" s="472" t="s">
+        <v>146</v>
+      </c>
+      <c r="G276" s="430" t="s">
         <v>145</v>
       </c>
-      <c r="H276" s="458" t="s">
-        <v>147</v>
-      </c>
-      <c r="I276" s="457">
-        <v>11</v>
-      </c>
-      <c r="J276" s="457"/>
-      <c r="K276" s="459"/>
+      <c r="H276" s="462" t="s">
+        <v>148</v>
+      </c>
+      <c r="I276" s="472">
+        <v>256</v>
+      </c>
+      <c r="J276" s="463"/>
+      <c r="K276" s="477"/>
       <c r="L276" s="422"/>
       <c r="M276" s="422"/>
       <c r="N276" s="422"/>
@@ -25725,99 +25772,702 @@
       <c r="B277" s="428">
         <v>11</v>
       </c>
-      <c r="C277" s="449" t="s">
-        <v>155</v>
-      </c>
-      <c r="D277" s="449" t="s">
-        <v>160</v>
+      <c r="C277" s="462" t="s">
+        <v>325</v>
+      </c>
+      <c r="D277" s="462" t="s">
+        <v>328</v>
       </c>
       <c r="E277" s="430" t="s">
         <v>146</v>
       </c>
-      <c r="F277" s="430" t="s">
-        <v>146</v>
-      </c>
-      <c r="G277" s="450" t="s">
+      <c r="F277" s="472" t="s">
+        <v>146</v>
+      </c>
+      <c r="G277" s="430" t="s">
         <v>145</v>
       </c>
-      <c r="H277" s="451" t="s">
+      <c r="H277" s="462" t="s">
         <v>148</v>
       </c>
-      <c r="I277" s="450">
+      <c r="I277" s="472">
         <v>256</v>
       </c>
-      <c r="J277" s="450"/>
-      <c r="K277" s="452"/>
+      <c r="J277" s="463"/>
+      <c r="K277" s="477"/>
       <c r="L277" s="422"/>
       <c r="M277" s="422"/>
       <c r="N277" s="422"/>
       <c r="O277" s="424"/>
     </row>
     <row r="278" spans="1:15" s="421" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A278" s="422"/>
+      <c r="A278" s="423"/>
       <c r="B278" s="428">
         <v>12</v>
       </c>
-      <c r="C278" s="449" t="s">
-        <v>156</v>
-      </c>
-      <c r="D278" s="449" t="s">
-        <v>158</v>
+      <c r="C278" s="462" t="s">
+        <v>326</v>
+      </c>
+      <c r="D278" s="462" t="s">
+        <v>329</v>
       </c>
       <c r="E278" s="430" t="s">
         <v>146</v>
       </c>
-      <c r="F278" s="430" t="s">
-        <v>146</v>
-      </c>
-      <c r="G278" s="450" t="s">
-        <v>146</v>
-      </c>
-      <c r="H278" s="451" t="s">
-        <v>147</v>
-      </c>
-      <c r="I278" s="450">
-        <v>11</v>
-      </c>
-      <c r="J278" s="450"/>
-      <c r="K278" s="452"/>
+      <c r="F278" s="472" t="s">
+        <v>146</v>
+      </c>
+      <c r="G278" s="430" t="s">
+        <v>145</v>
+      </c>
+      <c r="H278" s="462" t="s">
+        <v>148</v>
+      </c>
+      <c r="I278" s="472">
+        <v>256</v>
+      </c>
+      <c r="J278" s="463"/>
+      <c r="K278" s="477"/>
       <c r="L278" s="422"/>
       <c r="M278" s="422"/>
       <c r="N278" s="422"/>
       <c r="O278" s="424"/>
     </row>
-    <row r="279" spans="1:15" s="421" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="279" spans="1:15" s="421" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A279" s="423"/>
-      <c r="B279" s="434">
+      <c r="B279" s="428">
         <v>13</v>
       </c>
-      <c r="C279" s="435" t="s">
-        <v>157</v>
-      </c>
-      <c r="D279" s="435" t="s">
-        <v>161</v>
-      </c>
-      <c r="E279" s="436" t="s">
-        <v>146</v>
-      </c>
-      <c r="F279" s="436" t="s">
-        <v>146</v>
-      </c>
-      <c r="G279" s="436" t="s">
-        <v>146</v>
-      </c>
-      <c r="H279" s="437" t="s">
-        <v>148</v>
-      </c>
-      <c r="I279" s="436">
-        <v>256</v>
-      </c>
-      <c r="J279" s="436"/>
-      <c r="K279" s="438"/>
+      <c r="C279" s="429" t="s">
+        <v>166</v>
+      </c>
+      <c r="D279" s="429" t="s">
+        <v>167</v>
+      </c>
+      <c r="E279" s="430" t="s">
+        <v>146</v>
+      </c>
+      <c r="F279" s="430" t="s">
+        <v>146</v>
+      </c>
+      <c r="G279" s="430" t="s">
+        <v>145</v>
+      </c>
+      <c r="H279" s="431" t="s">
+        <v>147</v>
+      </c>
+      <c r="I279" s="430">
+        <v>11</v>
+      </c>
+      <c r="J279" s="430"/>
+      <c r="K279" s="288" t="s">
+        <v>168</v>
+      </c>
       <c r="L279" s="422"/>
       <c r="M279" s="422"/>
       <c r="N279" s="422"/>
       <c r="O279" s="424"/>
+    </row>
+    <row r="280" spans="1:15" s="421" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A280" s="465"/>
+      <c r="B280" s="428">
+        <v>14</v>
+      </c>
+      <c r="C280" s="456" t="s">
+        <v>154</v>
+      </c>
+      <c r="D280" s="456" t="s">
+        <v>159</v>
+      </c>
+      <c r="E280" s="430" t="s">
+        <v>146</v>
+      </c>
+      <c r="F280" s="430" t="s">
+        <v>146</v>
+      </c>
+      <c r="G280" s="457" t="s">
+        <v>145</v>
+      </c>
+      <c r="H280" s="458" t="s">
+        <v>148</v>
+      </c>
+      <c r="I280" s="457">
+        <v>10</v>
+      </c>
+      <c r="J280" s="457"/>
+      <c r="K280" s="459"/>
+      <c r="L280" s="422"/>
+      <c r="M280" s="422"/>
+      <c r="N280" s="422"/>
+      <c r="O280" s="424"/>
+    </row>
+    <row r="281" spans="1:15" s="421" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A281" s="423"/>
+      <c r="B281" s="428">
+        <v>15</v>
+      </c>
+      <c r="C281" s="449" t="s">
+        <v>155</v>
+      </c>
+      <c r="D281" s="449" t="s">
+        <v>160</v>
+      </c>
+      <c r="E281" s="430" t="s">
+        <v>146</v>
+      </c>
+      <c r="F281" s="430" t="s">
+        <v>146</v>
+      </c>
+      <c r="G281" s="450" t="s">
+        <v>145</v>
+      </c>
+      <c r="H281" s="451" t="s">
+        <v>148</v>
+      </c>
+      <c r="I281" s="450">
+        <v>256</v>
+      </c>
+      <c r="J281" s="450"/>
+      <c r="K281" s="452"/>
+      <c r="L281" s="422"/>
+      <c r="M281" s="422"/>
+      <c r="N281" s="422"/>
+      <c r="O281" s="424"/>
+    </row>
+    <row r="282" spans="1:15" s="421" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A282" s="422"/>
+      <c r="B282" s="428">
+        <v>16</v>
+      </c>
+      <c r="C282" s="449" t="s">
+        <v>156</v>
+      </c>
+      <c r="D282" s="449" t="s">
+        <v>158</v>
+      </c>
+      <c r="E282" s="430" t="s">
+        <v>146</v>
+      </c>
+      <c r="F282" s="430" t="s">
+        <v>146</v>
+      </c>
+      <c r="G282" s="450" t="s">
+        <v>146</v>
+      </c>
+      <c r="H282" s="451" t="s">
+        <v>147</v>
+      </c>
+      <c r="I282" s="450">
+        <v>11</v>
+      </c>
+      <c r="J282" s="450"/>
+      <c r="K282" s="452"/>
+      <c r="L282" s="422"/>
+      <c r="M282" s="422"/>
+      <c r="N282" s="422"/>
+      <c r="O282" s="424"/>
+    </row>
+    <row r="283" spans="1:15" s="421" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A283" s="423"/>
+      <c r="B283" s="434">
+        <v>17</v>
+      </c>
+      <c r="C283" s="435" t="s">
+        <v>157</v>
+      </c>
+      <c r="D283" s="435" t="s">
+        <v>161</v>
+      </c>
+      <c r="E283" s="436" t="s">
+        <v>146</v>
+      </c>
+      <c r="F283" s="436" t="s">
+        <v>146</v>
+      </c>
+      <c r="G283" s="436" t="s">
+        <v>146</v>
+      </c>
+      <c r="H283" s="437" t="s">
+        <v>148</v>
+      </c>
+      <c r="I283" s="436">
+        <v>256</v>
+      </c>
+      <c r="J283" s="436"/>
+      <c r="K283" s="438"/>
+      <c r="L283" s="422"/>
+      <c r="M283" s="422"/>
+      <c r="N283" s="422"/>
+      <c r="O283" s="424"/>
+    </row>
+    <row r="286" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="287" spans="1:15" s="421" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A287" s="423"/>
+      <c r="B287" s="169" t="s">
+        <v>40</v>
+      </c>
+      <c r="C287" s="470"/>
+      <c r="D287" s="170" t="s">
+        <v>330</v>
+      </c>
+      <c r="E287" s="171"/>
+      <c r="F287" s="171"/>
+      <c r="G287" s="172"/>
+      <c r="H287" s="470"/>
+      <c r="I287" s="470"/>
+      <c r="J287" s="470"/>
+      <c r="K287" s="470"/>
+      <c r="L287" s="422"/>
+      <c r="M287" s="422"/>
+      <c r="N287" s="422"/>
+      <c r="O287" s="424"/>
+    </row>
+    <row r="288" spans="1:15" s="421" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A288" s="423"/>
+      <c r="B288" s="422"/>
+      <c r="C288" s="422"/>
+      <c r="D288" s="422"/>
+      <c r="E288" s="422"/>
+      <c r="F288" s="422"/>
+      <c r="G288" s="422"/>
+      <c r="H288" s="422"/>
+      <c r="I288" s="422"/>
+      <c r="J288" s="422"/>
+      <c r="K288" s="422"/>
+      <c r="L288" s="422"/>
+      <c r="M288" s="422"/>
+      <c r="N288" s="422"/>
+      <c r="O288" s="424"/>
+    </row>
+    <row r="289" spans="1:15" s="421" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A289" s="423"/>
+      <c r="B289" s="425" t="s">
+        <v>0</v>
+      </c>
+      <c r="C289" s="426" t="s">
+        <v>30</v>
+      </c>
+      <c r="D289" s="426" t="s">
+        <v>31</v>
+      </c>
+      <c r="E289" s="426" t="s">
+        <v>32</v>
+      </c>
+      <c r="F289" s="426" t="s">
+        <v>33</v>
+      </c>
+      <c r="G289" s="426" t="s">
+        <v>34</v>
+      </c>
+      <c r="H289" s="426" t="s">
+        <v>35</v>
+      </c>
+      <c r="I289" s="426" t="s">
+        <v>36</v>
+      </c>
+      <c r="J289" s="426" t="s">
+        <v>37</v>
+      </c>
+      <c r="K289" s="427" t="s">
+        <v>38</v>
+      </c>
+      <c r="L289" s="422"/>
+      <c r="M289" s="422"/>
+      <c r="N289" s="422"/>
+      <c r="O289" s="424"/>
+    </row>
+    <row r="290" spans="1:15" s="421" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B290" s="473">
+        <v>1</v>
+      </c>
+      <c r="C290" s="474" t="s">
+        <v>239</v>
+      </c>
+      <c r="D290" s="474" t="s">
+        <v>240</v>
+      </c>
+      <c r="E290" s="476" t="s">
+        <v>145</v>
+      </c>
+      <c r="F290" s="476" t="s">
+        <v>145</v>
+      </c>
+      <c r="G290" s="476" t="s">
+        <v>145</v>
+      </c>
+      <c r="H290" s="474" t="s">
+        <v>147</v>
+      </c>
+      <c r="I290" s="476">
+        <v>11</v>
+      </c>
+      <c r="J290" s="474"/>
+      <c r="K290" s="475"/>
+    </row>
+    <row r="291" spans="1:15" s="421" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A291" s="465"/>
+      <c r="B291" s="276">
+        <v>2</v>
+      </c>
+      <c r="C291" s="429" t="s">
+        <v>334</v>
+      </c>
+      <c r="D291" s="429" t="s">
+        <v>331</v>
+      </c>
+      <c r="E291" s="430" t="s">
+        <v>146</v>
+      </c>
+      <c r="F291" s="430" t="s">
+        <v>146</v>
+      </c>
+      <c r="G291" s="430" t="s">
+        <v>145</v>
+      </c>
+      <c r="H291" s="431" t="s">
+        <v>148</v>
+      </c>
+      <c r="I291" s="430">
+        <v>256</v>
+      </c>
+      <c r="J291" s="430"/>
+      <c r="K291" s="452"/>
+      <c r="L291" s="470"/>
+      <c r="M291" s="422"/>
+      <c r="N291" s="422"/>
+      <c r="O291" s="424"/>
+    </row>
+    <row r="292" spans="1:15" s="421" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A292" s="465"/>
+      <c r="B292" s="276">
+        <v>3</v>
+      </c>
+      <c r="C292" s="462" t="s">
+        <v>335</v>
+      </c>
+      <c r="D292" s="462" t="s">
+        <v>315</v>
+      </c>
+      <c r="E292" s="430" t="s">
+        <v>146</v>
+      </c>
+      <c r="F292" s="472" t="s">
+        <v>146</v>
+      </c>
+      <c r="G292" s="430" t="s">
+        <v>145</v>
+      </c>
+      <c r="H292" s="431" t="s">
+        <v>148</v>
+      </c>
+      <c r="I292" s="430">
+        <v>256</v>
+      </c>
+      <c r="J292" s="574"/>
+      <c r="K292" s="452"/>
+      <c r="L292" s="470"/>
+      <c r="M292" s="422"/>
+      <c r="N292" s="422"/>
+      <c r="O292" s="424"/>
+    </row>
+    <row r="293" spans="1:15" s="421" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A293" s="465"/>
+      <c r="B293" s="276">
+        <v>4</v>
+      </c>
+      <c r="C293" s="462" t="s">
+        <v>310</v>
+      </c>
+      <c r="D293" s="462" t="s">
+        <v>316</v>
+      </c>
+      <c r="E293" s="430" t="s">
+        <v>146</v>
+      </c>
+      <c r="F293" s="472" t="s">
+        <v>146</v>
+      </c>
+      <c r="G293" s="430" t="s">
+        <v>145</v>
+      </c>
+      <c r="H293" s="431" t="s">
+        <v>148</v>
+      </c>
+      <c r="I293" s="430">
+        <v>256</v>
+      </c>
+      <c r="J293" s="574"/>
+      <c r="K293" s="452"/>
+      <c r="L293" s="470"/>
+      <c r="M293" s="422"/>
+      <c r="N293" s="422"/>
+      <c r="O293" s="424"/>
+    </row>
+    <row r="294" spans="1:15" s="421" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A294" s="423"/>
+      <c r="B294" s="428">
+        <v>5</v>
+      </c>
+      <c r="C294" s="462" t="s">
+        <v>283</v>
+      </c>
+      <c r="D294" s="462" t="s">
+        <v>285</v>
+      </c>
+      <c r="E294" s="430" t="s">
+        <v>146</v>
+      </c>
+      <c r="F294" s="472" t="s">
+        <v>146</v>
+      </c>
+      <c r="G294" s="430" t="s">
+        <v>145</v>
+      </c>
+      <c r="H294" s="462" t="s">
+        <v>148</v>
+      </c>
+      <c r="I294" s="472">
+        <v>256</v>
+      </c>
+      <c r="J294" s="463"/>
+      <c r="K294" s="464"/>
+      <c r="L294" s="422"/>
+      <c r="M294" s="422"/>
+      <c r="N294" s="422"/>
+      <c r="O294" s="424"/>
+    </row>
+    <row r="295" spans="1:15" s="421" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A295" s="423"/>
+      <c r="B295" s="461">
+        <v>6</v>
+      </c>
+      <c r="C295" s="462" t="s">
+        <v>284</v>
+      </c>
+      <c r="D295" s="462" t="s">
+        <v>286</v>
+      </c>
+      <c r="E295" s="430" t="s">
+        <v>146</v>
+      </c>
+      <c r="F295" s="472" t="s">
+        <v>146</v>
+      </c>
+      <c r="G295" s="430" t="s">
+        <v>145</v>
+      </c>
+      <c r="H295" s="462" t="s">
+        <v>148</v>
+      </c>
+      <c r="I295" s="472">
+        <v>256</v>
+      </c>
+      <c r="J295" s="463"/>
+      <c r="K295" s="464"/>
+      <c r="L295" s="422"/>
+      <c r="M295" s="422"/>
+      <c r="N295" s="422"/>
+      <c r="O295" s="424"/>
+    </row>
+    <row r="296" spans="1:15" s="421" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A296" s="423"/>
+      <c r="B296" s="461">
+        <v>7</v>
+      </c>
+      <c r="C296" s="462" t="s">
+        <v>332</v>
+      </c>
+      <c r="D296" s="462" t="s">
+        <v>333</v>
+      </c>
+      <c r="E296" s="430" t="s">
+        <v>146</v>
+      </c>
+      <c r="F296" s="472" t="s">
+        <v>146</v>
+      </c>
+      <c r="G296" s="430" t="s">
+        <v>145</v>
+      </c>
+      <c r="H296" s="462" t="s">
+        <v>148</v>
+      </c>
+      <c r="I296" s="472">
+        <v>20</v>
+      </c>
+      <c r="J296" s="463"/>
+      <c r="K296" s="464"/>
+      <c r="L296" s="422"/>
+      <c r="M296" s="422"/>
+      <c r="N296" s="422"/>
+      <c r="O296" s="424"/>
+    </row>
+    <row r="297" spans="1:15" s="421" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A297" s="465"/>
+      <c r="B297" s="428">
+        <v>8</v>
+      </c>
+      <c r="C297" s="429" t="s">
+        <v>166</v>
+      </c>
+      <c r="D297" s="429" t="s">
+        <v>167</v>
+      </c>
+      <c r="E297" s="430" t="s">
+        <v>146</v>
+      </c>
+      <c r="F297" s="430" t="s">
+        <v>146</v>
+      </c>
+      <c r="G297" s="430" t="s">
+        <v>145</v>
+      </c>
+      <c r="H297" s="431" t="s">
+        <v>147</v>
+      </c>
+      <c r="I297" s="430">
+        <v>11</v>
+      </c>
+      <c r="J297" s="430"/>
+      <c r="K297" s="288" t="s">
+        <v>168</v>
+      </c>
+      <c r="L297" s="470"/>
+      <c r="M297" s="470"/>
+      <c r="N297" s="470"/>
+      <c r="O297" s="471"/>
+    </row>
+    <row r="298" spans="1:15" s="421" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A298" s="423"/>
+      <c r="B298" s="428">
+        <v>9</v>
+      </c>
+      <c r="C298" s="456" t="s">
+        <v>154</v>
+      </c>
+      <c r="D298" s="456" t="s">
+        <v>159</v>
+      </c>
+      <c r="E298" s="430" t="s">
+        <v>146</v>
+      </c>
+      <c r="F298" s="430" t="s">
+        <v>146</v>
+      </c>
+      <c r="G298" s="457" t="s">
+        <v>145</v>
+      </c>
+      <c r="H298" s="458" t="s">
+        <v>148</v>
+      </c>
+      <c r="I298" s="457">
+        <v>10</v>
+      </c>
+      <c r="J298" s="457"/>
+      <c r="K298" s="459"/>
+      <c r="L298" s="422"/>
+      <c r="M298" s="422"/>
+      <c r="N298" s="422"/>
+      <c r="O298" s="424"/>
+    </row>
+    <row r="299" spans="1:15" s="421" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A299" s="422"/>
+      <c r="B299" s="428">
+        <v>10</v>
+      </c>
+      <c r="C299" s="449" t="s">
+        <v>155</v>
+      </c>
+      <c r="D299" s="449" t="s">
+        <v>160</v>
+      </c>
+      <c r="E299" s="430" t="s">
+        <v>146</v>
+      </c>
+      <c r="F299" s="430" t="s">
+        <v>146</v>
+      </c>
+      <c r="G299" s="450" t="s">
+        <v>145</v>
+      </c>
+      <c r="H299" s="451" t="s">
+        <v>148</v>
+      </c>
+      <c r="I299" s="450">
+        <v>256</v>
+      </c>
+      <c r="J299" s="450"/>
+      <c r="K299" s="452"/>
+      <c r="L299" s="422"/>
+      <c r="M299" s="422"/>
+      <c r="N299" s="422"/>
+      <c r="O299" s="424"/>
+    </row>
+    <row r="300" spans="1:15" s="421" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A300" s="422"/>
+      <c r="B300" s="428">
+        <v>11</v>
+      </c>
+      <c r="C300" s="449" t="s">
+        <v>156</v>
+      </c>
+      <c r="D300" s="449" t="s">
+        <v>158</v>
+      </c>
+      <c r="E300" s="430" t="s">
+        <v>146</v>
+      </c>
+      <c r="F300" s="430" t="s">
+        <v>146</v>
+      </c>
+      <c r="G300" s="450" t="s">
+        <v>146</v>
+      </c>
+      <c r="H300" s="451" t="s">
+        <v>147</v>
+      </c>
+      <c r="I300" s="450">
+        <v>11</v>
+      </c>
+      <c r="J300" s="450"/>
+      <c r="K300" s="452"/>
+      <c r="L300" s="422"/>
+      <c r="M300" s="422"/>
+      <c r="N300" s="422"/>
+      <c r="O300" s="424"/>
+    </row>
+    <row r="301" spans="1:15" s="421" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A301" s="423"/>
+      <c r="B301" s="434">
+        <v>12</v>
+      </c>
+      <c r="C301" s="435" t="s">
+        <v>157</v>
+      </c>
+      <c r="D301" s="435" t="s">
+        <v>161</v>
+      </c>
+      <c r="E301" s="436" t="s">
+        <v>146</v>
+      </c>
+      <c r="F301" s="436" t="s">
+        <v>146</v>
+      </c>
+      <c r="G301" s="436" t="s">
+        <v>146</v>
+      </c>
+      <c r="H301" s="437" t="s">
+        <v>148</v>
+      </c>
+      <c r="I301" s="436">
+        <v>256</v>
+      </c>
+      <c r="J301" s="436"/>
+      <c r="K301" s="438"/>
+      <c r="L301" s="422"/>
+      <c r="M301" s="422"/>
+      <c r="N301" s="422"/>
+      <c r="O301" s="424"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Replace 100% each excel page
</commit_message>
<xml_diff>
--- a/02.DesignDocument/Project_Management.xlsx
+++ b/02.DesignDocument/Project_Management.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\yadanar_thike\02.DesignDocument\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PHP\htdocs\YadnarThike\02.DesignDocument\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15AB7994-4D3D-43F2-88FC-9A85C2183930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="3" r:id="rId1"/>
@@ -26,7 +25,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="5">'DB Design'!$A$1:$O$350</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Schedule!$A$1:$O$112</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1179,7 +1178,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -3063,8 +3062,8 @@
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal 2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 2 2" xfId="4"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3100,7 +3099,7 @@
         <xdr:cNvPr id="2" name="Rectangle: Rounded Corners 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AEF0383-2F02-5166-046E-39160DBF55AA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9AEF0383-2F02-5166-046E-39160DBF55AA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3163,7 +3162,7 @@
         <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DA2F3EC-D7CC-A755-7F92-8A981AAE9ED8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8DA2F3EC-D7CC-A755-7F92-8A981AAE9ED8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3220,7 +3219,7 @@
         <xdr:cNvPr id="14" name="Rectangle 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{885A1CB4-BB53-8D25-DB6A-12ED4759F1B4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{885A1CB4-BB53-8D25-DB6A-12ED4759F1B4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3283,7 +3282,7 @@
         <xdr:cNvPr id="87" name="Rectangle 86">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F94611E8-1812-5B4C-017A-153E4C34388C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F94611E8-1812-5B4C-017A-153E4C34388C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3346,7 +3345,7 @@
         <xdr:cNvPr id="114" name="Diamond 113">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C7364F4-7338-69BA-F34F-B050A32D9C97}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5C7364F4-7338-69BA-F34F-B050A32D9C97}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3414,7 +3413,7 @@
         <xdr:cNvPr id="123" name="Straight Arrow Connector 122">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF22D1DA-2F78-797E-4E09-2767EFDFA1E1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DF22D1DA-2F78-797E-4E09-2767EFDFA1E1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3470,7 +3469,7 @@
         <xdr:cNvPr id="202" name="Rectangle 201">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{376418BB-84E2-9783-C488-B78334DD1F04}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{376418BB-84E2-9783-C488-B78334DD1F04}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3533,7 +3532,7 @@
         <xdr:cNvPr id="145" name="Rectangle 144">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52AB3D84-7233-AFDC-86BC-8C5B16D136C0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{52AB3D84-7233-AFDC-86BC-8C5B16D136C0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3601,7 +3600,7 @@
         <xdr:cNvPr id="147" name="Straight Arrow Connector 146">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E11A7598-E628-B6B6-0F75-4F9E47A60D7B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E11A7598-E628-B6B6-0F75-4F9E47A60D7B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3657,7 +3656,7 @@
         <xdr:cNvPr id="222" name="Rectangle 221">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E0DB5F9-7626-347E-EBB3-AC8A13B46077}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7E0DB5F9-7626-347E-EBB3-AC8A13B46077}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3720,7 +3719,7 @@
         <xdr:cNvPr id="223" name="Rectangle 222">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C9AB86F-F0A4-7508-3245-97E1F51BF0C8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5C9AB86F-F0A4-7508-3245-97E1F51BF0C8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3783,7 +3782,7 @@
         <xdr:cNvPr id="224" name="Rectangle 223">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43C650F7-26B8-AF80-8936-0D65794F54C0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{43C650F7-26B8-AF80-8936-0D65794F54C0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3846,7 +3845,7 @@
         <xdr:cNvPr id="225" name="Rectangle 224">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{563FE4EC-AED3-BDE2-9E0A-2DED8435744C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{563FE4EC-AED3-BDE2-9E0A-2DED8435744C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3909,7 +3908,7 @@
         <xdr:cNvPr id="226" name="Rectangle 225">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43293255-1E5C-6D64-B6B5-4C534012B38A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{43293255-1E5C-6D64-B6B5-4C534012B38A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3972,7 +3971,7 @@
         <xdr:cNvPr id="200" name="Straight Arrow Connector 199">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6742F96-6706-4F25-2402-16D113F50115}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A6742F96-6706-4F25-2402-16D113F50115}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4028,7 +4027,7 @@
         <xdr:cNvPr id="203" name="Connector: Elbow 202">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C05F93F-4491-1089-9C75-95522BE2D55F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3C05F93F-4491-1089-9C75-95522BE2D55F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4084,7 +4083,7 @@
         <xdr:cNvPr id="204" name="Rectangle 203">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CC39AC3-D31A-3DEB-3FA3-30B6E9970945}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2CC39AC3-D31A-3DEB-3FA3-30B6E9970945}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4154,7 +4153,7 @@
         <xdr:cNvPr id="277" name="Rectangle 276">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9756E1D-6F8D-1F73-125B-283F0DE30E65}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A9756E1D-6F8D-1F73-125B-283F0DE30E65}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4238,7 +4237,7 @@
         <xdr:cNvPr id="291" name="Rectangle 290">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF98E191-C7E4-E3CC-8C70-430CA3D8877C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BF98E191-C7E4-E3CC-8C70-430CA3D8877C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4301,7 +4300,7 @@
         <xdr:cNvPr id="293" name="Rectangle 292">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A0868AF-0480-E151-77F7-48BBCAD87EBE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4A0868AF-0480-E151-77F7-48BBCAD87EBE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4369,7 +4368,7 @@
         <xdr:cNvPr id="300" name="Rectangle 299">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E6E3BFD-0229-1CE5-EE43-A63860D12EBE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6E6E3BFD-0229-1CE5-EE43-A63860D12EBE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4451,7 +4450,7 @@
         <xdr:cNvPr id="301" name="Rectangle 300">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DCF44B1-E01B-8F32-6664-957E27134710}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8DCF44B1-E01B-8F32-6664-957E27134710}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4526,7 +4525,7 @@
         <xdr:cNvPr id="302" name="Rectangle 301">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D146A799-3F91-BEA2-C4AC-70D0BFB81705}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D146A799-3F91-BEA2-C4AC-70D0BFB81705}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4596,7 +4595,7 @@
         <xdr:cNvPr id="303" name="Rectangle 302">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D11C16C0-C18D-908F-0C8F-19BD003ADB1A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D11C16C0-C18D-908F-0C8F-19BD003ADB1A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4688,7 +4687,7 @@
         <xdr:cNvPr id="304" name="Rectangle 303">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38825BBC-E7DA-8E56-346A-DDBBD3BFB779}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{38825BBC-E7DA-8E56-346A-DDBBD3BFB779}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4836,7 +4835,7 @@
         <xdr:cNvPr id="237" name="Straight Arrow Connector 236">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{037BC34B-6C53-3788-40A5-DAC45ED79BB9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{037BC34B-6C53-3788-40A5-DAC45ED79BB9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4892,7 +4891,7 @@
         <xdr:cNvPr id="239" name="Straight Arrow Connector 238">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CE8FD69-B553-CCDC-31AA-09D8966076F0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7CE8FD69-B553-CCDC-31AA-09D8966076F0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4948,7 +4947,7 @@
         <xdr:cNvPr id="241" name="Straight Arrow Connector 240">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1C676F3-8BEF-A082-3DD6-F6AD8E75064A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E1C676F3-8BEF-A082-3DD6-F6AD8E75064A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5004,7 +5003,7 @@
         <xdr:cNvPr id="245" name="Straight Arrow Connector 244">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1D134DC-5B05-FA17-30E8-2C3E2062CA13}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C1D134DC-5B05-FA17-30E8-2C3E2062CA13}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5060,7 +5059,7 @@
         <xdr:cNvPr id="247" name="Straight Arrow Connector 246">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00161F50-D4EE-ED6B-BC73-FCE6E53DAA69}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00161F50-D4EE-ED6B-BC73-FCE6E53DAA69}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5116,7 +5115,7 @@
         <xdr:cNvPr id="249" name="Straight Arrow Connector 248">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A9250D8-1B9A-5DF4-B5F1-5B12D556DAE9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5A9250D8-1B9A-5DF4-B5F1-5B12D556DAE9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5172,7 +5171,7 @@
         <xdr:cNvPr id="252" name="Straight Arrow Connector 251">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F22E0AB-0901-8AF5-3AF6-5531E8346140}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4F22E0AB-0901-8AF5-3AF6-5531E8346140}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5228,7 +5227,7 @@
         <xdr:cNvPr id="344" name="Rectangle 343">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15C556D5-CFE2-5B92-F0B7-618EA2C8C2C3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{15C556D5-CFE2-5B92-F0B7-618EA2C8C2C3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5291,7 +5290,7 @@
         <xdr:cNvPr id="272" name="Straight Arrow Connector 271">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D3A92E1-E68B-2036-35C8-C08772D9A190}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7D3A92E1-E68B-2036-35C8-C08772D9A190}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5347,7 +5346,7 @@
         <xdr:cNvPr id="348" name="Rectangle 347">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B4943A5-87A8-8961-F71B-CF985DA7737F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4B4943A5-87A8-8961-F71B-CF985DA7737F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5410,7 +5409,7 @@
         <xdr:cNvPr id="349" name="Rectangle 348">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE70EF5F-57EE-538D-1A2B-6CE761C2A3EC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AE70EF5F-57EE-538D-1A2B-6CE761C2A3EC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5473,7 +5472,7 @@
         <xdr:cNvPr id="350" name="Rectangle 349">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FD6BAA2-6530-2210-8E3E-BEE408084FE2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5FD6BAA2-6530-2210-8E3E-BEE408084FE2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5541,7 +5540,7 @@
         <xdr:cNvPr id="353" name="Rectangle 352">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0CF8AB2-E6DF-7400-C8D1-D71662BA4395}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0CF8AB2-E6DF-7400-C8D1-D71662BA4395}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5604,7 +5603,7 @@
         <xdr:cNvPr id="354" name="Rectangle 353">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC19F654-D768-AED9-5333-191F663C8E48}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EC19F654-D768-AED9-5333-191F663C8E48}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5667,7 +5666,7 @@
         <xdr:cNvPr id="275" name="Connector: Elbow 274">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C9492A7-0C08-175E-FBA6-2D5CB2631358}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9C9492A7-0C08-175E-FBA6-2D5CB2631358}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5723,7 +5722,7 @@
         <xdr:cNvPr id="284" name="Connector: Elbow 283">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7FE5FB1-3A1D-BE07-BD5E-E9417CD08CAA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E7FE5FB1-3A1D-BE07-BD5E-E9417CD08CAA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5779,7 +5778,7 @@
         <xdr:cNvPr id="286" name="Connector: Elbow 285">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F891C8B-0021-74DF-749D-0D7841441398}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1F891C8B-0021-74DF-749D-0D7841441398}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5835,7 +5834,7 @@
         <xdr:cNvPr id="288" name="Connector: Elbow 287">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1F9DDA5-4B78-477C-6C18-243D1EF4BFDE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A1F9DDA5-4B78-477C-6C18-243D1EF4BFDE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5891,7 +5890,7 @@
         <xdr:cNvPr id="290" name="Connector: Elbow 289">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1666855-92A2-6E3D-DDEC-4E081B1D4307}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E1666855-92A2-6E3D-DDEC-4E081B1D4307}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5947,7 +5946,7 @@
         <xdr:cNvPr id="297" name="Connector: Elbow 296">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95F949F4-0904-BFEA-9154-26FFBB4FA87F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{95F949F4-0904-BFEA-9154-26FFBB4FA87F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6003,7 +6002,7 @@
         <xdr:cNvPr id="299" name="Connector: Elbow 298">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A9E6B12-2431-00DD-AA78-5479B0E4A645}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1A9E6B12-2431-00DD-AA78-5479B0E4A645}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6059,7 +6058,7 @@
         <xdr:cNvPr id="306" name="Connector: Elbow 305">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F167EA2F-C46A-908F-16D9-5A97EE7CC6BD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F167EA2F-C46A-908F-16D9-5A97EE7CC6BD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6115,7 +6114,7 @@
         <xdr:cNvPr id="308" name="Connector: Elbow 307">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B93CA3EE-65C6-1DA7-3F20-981F04EED772}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B93CA3EE-65C6-1DA7-3F20-981F04EED772}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6171,7 +6170,7 @@
         <xdr:cNvPr id="310" name="Connector: Elbow 309">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0B05704-F543-2E75-7D0D-FCDD5E4C8C86}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F0B05704-F543-2E75-7D0D-FCDD5E4C8C86}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6227,7 +6226,7 @@
         <xdr:cNvPr id="312" name="Straight Arrow Connector 311">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A0AABE3-E6BB-B42F-95EA-D67EE8E5D378}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7A0AABE3-E6BB-B42F-95EA-D67EE8E5D378}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6283,7 +6282,7 @@
         <xdr:cNvPr id="320" name="Straight Arrow Connector 319">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90354B19-6855-E0D8-680D-1E4105DF0482}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{90354B19-6855-E0D8-680D-1E4105DF0482}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6339,7 +6338,7 @@
         <xdr:cNvPr id="322" name="Rectangle 321">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A18F4F7C-87F5-DB03-151D-A83CCBEC56DA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A18F4F7C-87F5-DB03-151D-A83CCBEC56DA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6402,7 +6401,7 @@
         <xdr:cNvPr id="395" name="Rectangle 394">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EBD1FD7-007B-D887-47BA-DA775FEB2509}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8EBD1FD7-007B-D887-47BA-DA775FEB2509}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6465,7 +6464,7 @@
         <xdr:cNvPr id="396" name="Rectangle 395">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83417375-8D54-3374-22BD-906DEC74C681}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{83417375-8D54-3374-22BD-906DEC74C681}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6528,7 +6527,7 @@
         <xdr:cNvPr id="399" name="Rectangle 398">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7EBE78C-9D75-0F1B-994D-E45226229227}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F7EBE78C-9D75-0F1B-994D-E45226229227}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6596,7 +6595,7 @@
         <xdr:cNvPr id="402" name="Rectangle 401">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBFF531B-51DB-1F6D-EB96-AD7CC80D0F67}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BBFF531B-51DB-1F6D-EB96-AD7CC80D0F67}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6664,7 +6663,7 @@
         <xdr:cNvPr id="403" name="Rectangle 402">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C54CE03-4CBF-AB6C-446A-DFE119647AF5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8C54CE03-4CBF-AB6C-446A-DFE119647AF5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6732,7 +6731,7 @@
         <xdr:cNvPr id="324" name="Connector: Elbow 323">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B3106B3-9F5E-2D68-A93F-EAD98281AF68}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6B3106B3-9F5E-2D68-A93F-EAD98281AF68}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6790,7 +6789,7 @@
         <xdr:cNvPr id="326" name="Connector: Elbow 325">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A5A3CC7-F5E3-3A59-AAE6-5A77EF8AF76B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7A5A3CC7-F5E3-3A59-AAE6-5A77EF8AF76B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6848,7 +6847,7 @@
         <xdr:cNvPr id="328" name="Connector: Elbow 327">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59EA8637-5020-E5F2-74D2-94F1EF7FC222}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{59EA8637-5020-E5F2-74D2-94F1EF7FC222}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6906,7 +6905,7 @@
         <xdr:cNvPr id="330" name="Straight Arrow Connector 329">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B02CCDB-FA0B-72B0-A09C-FD22650E550C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2B02CCDB-FA0B-72B0-A09C-FD22650E550C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6962,7 +6961,7 @@
         <xdr:cNvPr id="333" name="Straight Arrow Connector 332">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A3EDF1A-1180-3DE2-F794-2034477DD130}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5A3EDF1A-1180-3DE2-F794-2034477DD130}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7018,7 +7017,7 @@
         <xdr:cNvPr id="336" name="Straight Arrow Connector 335">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D49E3D0B-1038-9898-7459-1899641E9168}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D49E3D0B-1038-9898-7459-1899641E9168}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7074,7 +7073,7 @@
         <xdr:cNvPr id="337" name="Diamond 336">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BEFA8B7-6CAC-A993-6CF5-2F9AE9E84215}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0BEFA8B7-6CAC-A993-6CF5-2F9AE9E84215}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7137,7 +7136,7 @@
         <xdr:cNvPr id="339" name="Straight Arrow Connector 338">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{031A5C72-A1A6-5D91-E183-A0A5BB5F4281}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{031A5C72-A1A6-5D91-E183-A0A5BB5F4281}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7193,7 +7192,7 @@
         <xdr:cNvPr id="345" name="Connector: Elbow 344">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1A60F90-7E17-D5BC-885D-93CF3719F5E5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E1A60F90-7E17-D5BC-885D-93CF3719F5E5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7249,7 +7248,7 @@
         <xdr:cNvPr id="357" name="Rectangle 356">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D4713C5-EDD9-4EA1-A109-F2489A23AA03}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5D4713C5-EDD9-4EA1-A109-F2489A23AA03}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7312,7 +7311,7 @@
         <xdr:cNvPr id="359" name="Straight Arrow Connector 358">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB0E2081-9AA7-67A9-D00B-7B6185BDEF36}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AB0E2081-9AA7-67A9-D00B-7B6185BDEF36}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7368,7 +7367,7 @@
         <xdr:cNvPr id="434" name="Rectangle 433">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{141C32BC-CF88-A0F0-A5FF-F2D39ECEE99A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{141C32BC-CF88-A0F0-A5FF-F2D39ECEE99A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7431,7 +7430,7 @@
         <xdr:cNvPr id="364" name="Connector: Elbow 363">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12FAF3DF-F9A7-21C4-6847-2432DF2AA5E8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{12FAF3DF-F9A7-21C4-6847-2432DF2AA5E8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7487,7 +7486,7 @@
         <xdr:cNvPr id="369" name="Straight Arrow Connector 368">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BA1F722-0166-8592-56C3-87D42892EE44}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0BA1F722-0166-8592-56C3-87D42892EE44}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7544,7 +7543,7 @@
         <xdr:cNvPr id="450" name="Rectangle 449">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{886D6DE6-1F36-FDA4-7903-597ECC919057}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{886D6DE6-1F36-FDA4-7903-597ECC919057}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7607,7 +7606,7 @@
         <xdr:cNvPr id="376" name="Straight Arrow Connector 375">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{064EF7AD-9F40-2DE8-EA0E-A5AD3E1983B5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{064EF7AD-9F40-2DE8-EA0E-A5AD3E1983B5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7664,7 +7663,7 @@
         <xdr:cNvPr id="464" name="Diamond 463">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C915F7B-BCE8-F060-1A20-20EB22B6006C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1C915F7B-BCE8-F060-1A20-20EB22B6006C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7735,7 +7734,7 @@
         <xdr:cNvPr id="454" name="Straight Arrow Connector 453">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E42FBB5-4535-71B8-FC68-8C7AFD6E4B7F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1E42FBB5-4535-71B8-FC68-8C7AFD6E4B7F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7792,7 +7791,7 @@
         <xdr:cNvPr id="461" name="Connector: Elbow 460">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E7714BA-E693-0D0A-6072-A8E598E8295E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4E7714BA-E693-0D0A-6072-A8E598E8295E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7848,7 +7847,7 @@
         <xdr:cNvPr id="478" name="Rectangle 477">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0212693D-D747-7775-BC2D-3520099979DA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0212693D-D747-7775-BC2D-3520099979DA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7911,7 +7910,7 @@
         <xdr:cNvPr id="482" name="Rectangle 481">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75D29002-7C66-2BC2-B0F6-DD3D754C32C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{75D29002-7C66-2BC2-B0F6-DD3D754C32C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7974,7 +7973,7 @@
         <xdr:cNvPr id="492" name="Rectangle 491">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41052F66-A624-F367-37B3-99FE9D72B420}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{41052F66-A624-F367-37B3-99FE9D72B420}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8037,7 +8036,7 @@
         <xdr:cNvPr id="481" name="Connector: Elbow 480">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A573981-F25B-1098-D017-0236FFF65BE8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7A573981-F25B-1098-D017-0236FFF65BE8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8093,7 +8092,7 @@
         <xdr:cNvPr id="488" name="Connector: Elbow 487">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49A0DB27-929E-5664-DD03-81AA2115F925}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{49A0DB27-929E-5664-DD03-81AA2115F925}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8149,7 +8148,7 @@
         <xdr:cNvPr id="503" name="Rectangle 502">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{634D115F-BA9D-AC73-8DC5-B177DA0DD039}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{634D115F-BA9D-AC73-8DC5-B177DA0DD039}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8212,7 +8211,7 @@
         <xdr:cNvPr id="504" name="Rectangle 503">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C8AF2C4-7266-FDA9-FE08-9BC163C40C03}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4C8AF2C4-7266-FDA9-FE08-9BC163C40C03}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8275,7 +8274,7 @@
         <xdr:cNvPr id="506" name="Rectangle 505">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2EBDBA8-B02C-6E11-A5CF-FA19199D9839}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B2EBDBA8-B02C-6E11-A5CF-FA19199D9839}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8338,7 +8337,7 @@
         <xdr:cNvPr id="493" name="Straight Arrow Connector 492">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C5F366E-B404-0BA8-F762-9F87E334EC57}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1C5F366E-B404-0BA8-F762-9F87E334EC57}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8394,7 +8393,7 @@
         <xdr:cNvPr id="496" name="Connector: Elbow 495">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A80C5828-9CA4-C951-9EC9-5C2405DB08ED}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A80C5828-9CA4-C951-9EC9-5C2405DB08ED}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8453,7 +8452,7 @@
         <xdr:cNvPr id="500" name="Connector: Elbow 499">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA55F324-FAA1-95C5-EDBB-B4F5BBF0B7B7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DA55F324-FAA1-95C5-EDBB-B4F5BBF0B7B7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8512,7 +8511,7 @@
         <xdr:cNvPr id="511" name="Connector: Elbow 510">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB2BDA04-D53F-E16F-40A1-938A443CB78D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FB2BDA04-D53F-E16F-40A1-938A443CB78D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8570,7 +8569,7 @@
         <xdr:cNvPr id="386" name="Connector: Elbow 385">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA2EA158-DD4C-9291-BFDE-414B28197C4B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EA2EA158-DD4C-9291-BFDE-414B28197C4B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8628,7 +8627,7 @@
         <xdr:cNvPr id="389" name="Connector: Elbow 388">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04FCD762-69B4-BDC9-5296-2856FFD8E380}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{04FCD762-69B4-BDC9-5296-2856FFD8E380}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8686,7 +8685,7 @@
         <xdr:cNvPr id="412" name="Straight Arrow Connector 411">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{214C2CBF-3AAB-DD40-58CA-B954AB2B953A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{214C2CBF-3AAB-DD40-58CA-B954AB2B953A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8742,7 +8741,7 @@
         <xdr:cNvPr id="549" name="Rectangle 548">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60EC7015-674F-C035-8A3D-90110260656A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{60EC7015-674F-C035-8A3D-90110260656A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8810,7 +8809,7 @@
         <xdr:cNvPr id="416" name="Connector: Elbow 415">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED0A8ADD-472B-E68A-3C0B-16A5345DF3E6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{ED0A8ADD-472B-E68A-3C0B-16A5345DF3E6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8866,7 +8865,7 @@
         <xdr:cNvPr id="557" name="Rectangle 556">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39EE8E70-69CA-73EB-081F-BFD537140F70}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{39EE8E70-69CA-73EB-081F-BFD537140F70}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8929,7 +8928,7 @@
         <xdr:cNvPr id="558" name="Rectangle 557">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30CE8806-D8D3-043E-346A-A936E52B704A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{30CE8806-D8D3-043E-346A-A936E52B704A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8992,7 +8991,7 @@
         <xdr:cNvPr id="559" name="Rectangle 558">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{234B76E3-C775-CB01-C51C-AE1B4C69027E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{234B76E3-C775-CB01-C51C-AE1B4C69027E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9060,7 +9059,7 @@
         <xdr:cNvPr id="560" name="Rectangle 559">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{472B8B14-8E1B-9E34-134D-077077E66926}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{472B8B14-8E1B-9E34-134D-077077E66926}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9123,7 +9122,7 @@
         <xdr:cNvPr id="561" name="Rectangle 560">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18A97039-056A-1BD6-2301-C7BB59A76C0F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{18A97039-056A-1BD6-2301-C7BB59A76C0F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9191,7 +9190,7 @@
         <xdr:cNvPr id="571" name="Rectangle 570">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E953785-7D8E-4AB8-5E1E-FA2F76927701}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5E953785-7D8E-4AB8-5E1E-FA2F76927701}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9259,7 +9258,7 @@
         <xdr:cNvPr id="429" name="Straight Arrow Connector 428">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CED1465-A771-205C-BBB6-126543509F4D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9CED1465-A771-205C-BBB6-126543509F4D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9315,7 +9314,7 @@
         <xdr:cNvPr id="431" name="Connector: Elbow 430">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{150A048A-D91E-76D5-513B-C8368E72C1B2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{150A048A-D91E-76D5-513B-C8368E72C1B2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9370,7 +9369,7 @@
         <xdr:cNvPr id="441" name="Connector: Elbow 440">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92A6C576-189D-57D5-C549-754EC4BF4FFB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{92A6C576-189D-57D5-C549-754EC4BF4FFB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9426,7 +9425,7 @@
         <xdr:cNvPr id="444" name="Connector: Elbow 443">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA5BD2F3-5151-9F42-96B2-B89822A7CB02}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BA5BD2F3-5151-9F42-96B2-B89822A7CB02}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9482,7 +9481,7 @@
         <xdr:cNvPr id="447" name="Straight Arrow Connector 446">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EA4DAB3-9587-14ED-27A9-B222D0C3BEE3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4EA4DAB3-9587-14ED-27A9-B222D0C3BEE3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9538,7 +9537,7 @@
         <xdr:cNvPr id="603" name="Rectangle 602">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A717D765-1050-685D-E446-A48827097EFD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A717D765-1050-685D-E446-A48827097EFD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9602,7 +9601,7 @@
         <xdr:cNvPr id="526" name="Connector: Elbow 525">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CCBB9D3-5B46-9C7E-1526-94F5B3F7D2E7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7CCBB9D3-5B46-9C7E-1526-94F5B3F7D2E7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9658,7 +9657,7 @@
         <xdr:cNvPr id="536" name="Connector: Elbow 535">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09CA61CF-1388-18BE-2EF6-C3AE83632FFA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{09CA61CF-1388-18BE-2EF6-C3AE83632FFA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9714,7 +9713,7 @@
         <xdr:cNvPr id="542" name="Connector: Elbow 541">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DB857A0-7AEE-F980-E064-1A06168B078B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9DB857A0-7AEE-F980-E064-1A06168B078B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9774,7 +9773,7 @@
         <xdr:cNvPr id="625" name="Rectangle 624">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{833FB374-0FE6-CB77-2438-275E7FD5493B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{833FB374-0FE6-CB77-2438-275E7FD5493B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9842,7 +9841,7 @@
         <xdr:cNvPr id="627" name="Rectangle 626">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAEA01B5-FF22-DD48-20CD-315D29C37784}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BAEA01B5-FF22-DD48-20CD-315D29C37784}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9905,7 +9904,7 @@
         <xdr:cNvPr id="565" name="Connector: Elbow 564">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{328480B0-0FBA-11FA-3C67-15DB6636684A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{328480B0-0FBA-11FA-3C67-15DB6636684A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9964,7 +9963,7 @@
         <xdr:cNvPr id="117" name="Rectangle 116">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{985192AB-8642-07F8-E04D-8EBAD661EEAF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{985192AB-8642-07F8-E04D-8EBAD661EEAF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10027,7 +10026,7 @@
         <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78333CFC-7F9C-DFFD-6398-476B4710F7FA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{78333CFC-7F9C-DFFD-6398-476B4710F7FA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10083,7 +10082,7 @@
         <xdr:cNvPr id="115" name="Rectangle 114">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED1F65BD-EFB7-BEFF-549F-9E4E36C12FAD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{ED1F65BD-EFB7-BEFF-549F-9E4E36C12FAD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10146,7 +10145,7 @@
         <xdr:cNvPr id="5" name="Connector: Elbow 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D31A361-7A62-F6FA-A055-24AA616A93D9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4D31A361-7A62-F6FA-A055-24AA616A93D9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10485,10 +10484,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11291,7 +11290,7 @@
       <c r="L48" s="540"/>
       <c r="M48" s="19">
         <f ca="1">NOW()</f>
-        <v>44704.409331712966</v>
+        <v>44704.549035185184</v>
       </c>
       <c r="N48" s="14"/>
     </row>
@@ -11312,7 +11311,7 @@
       <c r="L49" s="540"/>
       <c r="M49" s="19">
         <f ca="1">NOW()</f>
-        <v>44704.409331712966</v>
+        <v>44704.549035185184</v>
       </c>
       <c r="N49" s="14"/>
     </row>
@@ -11362,10 +11361,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q70"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12461,10 +12460,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O116"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="140" zoomScaleSheetLayoutView="70" workbookViewId="0"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="140" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -15710,10 +15709,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X82"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -17837,10 +17836,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q72"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -19225,7 +19224,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O348"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0"/>

</xml_diff>

<commit_message>
Task by person updated in the excel file
</commit_message>
<xml_diff>
--- a/02.DesignDocument/Project_Management.xlsx
+++ b/02.DesignDocument/Project_Management.xlsx
@@ -1,33 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\yadanar_thike\02.DesignDocument\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PHP\htdocs\YadnarThike\02.DesignDocument\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21F7A4CB-A7EB-42E1-BB35-54D5F69378BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="3" r:id="rId1"/>
     <sheet name="Customer Requirement" sheetId="9" r:id="rId2"/>
     <sheet name="Schedule" sheetId="1" r:id="rId3"/>
-    <sheet name="Main Flow" sheetId="2" r:id="rId4"/>
-    <sheet name="Screen Design" sheetId="4" r:id="rId5"/>
-    <sheet name="DB Design" sheetId="6" r:id="rId6"/>
+    <sheet name="By Person" sheetId="13" r:id="rId4"/>
+    <sheet name="Main Flow" sheetId="2" r:id="rId5"/>
+    <sheet name="Screen Design" sheetId="4" r:id="rId6"/>
+    <sheet name="DB Design" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'By Person'!$A$1:$U$16</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Cover!$A$1:$N$51</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Customer Requirement'!$A$1:$Q$70</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="5">'DB Design'!$A$1:$O$350</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">'DB Design'!$A$1:$O$350</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Schedule!$A$1:$O$112</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">'Screen Design'!$A$1:$Q$167</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">'Screen Design'!$A$1:$Q$167</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1967" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1984" uniqueCount="383">
   <si>
     <t>No</t>
   </si>
@@ -1181,12 +1182,30 @@
   </si>
   <si>
     <t>Privacy &amp; Policy</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Thet Htein Lin</t>
+  </si>
+  <si>
+    <t>Project Flow</t>
+  </si>
+  <si>
+    <t>DB Design</t>
+  </si>
+  <si>
+    <t>Screen Design</t>
+  </si>
+  <si>
+    <t>Design Development</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -1361,7 +1380,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1425,6 +1444,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2082,7 +2107,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="578">
+  <cellXfs count="601">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2970,6 +2995,15 @@
     <xf numFmtId="1" fontId="4" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="4" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3074,21 +3108,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="10" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal 2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 2 2" xfId="4"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3124,7 +3200,7 @@
         <xdr:cNvPr id="2" name="Rectangle: Rounded Corners 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AEF0383-2F02-5166-046E-39160DBF55AA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9AEF0383-2F02-5166-046E-39160DBF55AA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3187,7 +3263,7 @@
         <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DA2F3EC-D7CC-A755-7F92-8A981AAE9ED8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8DA2F3EC-D7CC-A755-7F92-8A981AAE9ED8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3244,7 +3320,7 @@
         <xdr:cNvPr id="14" name="Rectangle 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{885A1CB4-BB53-8D25-DB6A-12ED4759F1B4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{885A1CB4-BB53-8D25-DB6A-12ED4759F1B4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3307,7 +3383,7 @@
         <xdr:cNvPr id="87" name="Rectangle 86">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F94611E8-1812-5B4C-017A-153E4C34388C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F94611E8-1812-5B4C-017A-153E4C34388C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3370,7 +3446,7 @@
         <xdr:cNvPr id="114" name="Diamond 113">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C7364F4-7338-69BA-F34F-B050A32D9C97}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5C7364F4-7338-69BA-F34F-B050A32D9C97}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3438,7 +3514,7 @@
         <xdr:cNvPr id="123" name="Straight Arrow Connector 122">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF22D1DA-2F78-797E-4E09-2767EFDFA1E1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DF22D1DA-2F78-797E-4E09-2767EFDFA1E1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3494,7 +3570,7 @@
         <xdr:cNvPr id="202" name="Rectangle 201">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{376418BB-84E2-9783-C488-B78334DD1F04}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{376418BB-84E2-9783-C488-B78334DD1F04}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3557,7 +3633,7 @@
         <xdr:cNvPr id="145" name="Rectangle 144">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52AB3D84-7233-AFDC-86BC-8C5B16D136C0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{52AB3D84-7233-AFDC-86BC-8C5B16D136C0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3625,7 +3701,7 @@
         <xdr:cNvPr id="147" name="Straight Arrow Connector 146">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E11A7598-E628-B6B6-0F75-4F9E47A60D7B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E11A7598-E628-B6B6-0F75-4F9E47A60D7B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3681,7 +3757,7 @@
         <xdr:cNvPr id="222" name="Rectangle 221">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E0DB5F9-7626-347E-EBB3-AC8A13B46077}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7E0DB5F9-7626-347E-EBB3-AC8A13B46077}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3744,7 +3820,7 @@
         <xdr:cNvPr id="223" name="Rectangle 222">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C9AB86F-F0A4-7508-3245-97E1F51BF0C8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5C9AB86F-F0A4-7508-3245-97E1F51BF0C8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3807,7 +3883,7 @@
         <xdr:cNvPr id="224" name="Rectangle 223">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43C650F7-26B8-AF80-8936-0D65794F54C0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{43C650F7-26B8-AF80-8936-0D65794F54C0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3870,7 +3946,7 @@
         <xdr:cNvPr id="225" name="Rectangle 224">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{563FE4EC-AED3-BDE2-9E0A-2DED8435744C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{563FE4EC-AED3-BDE2-9E0A-2DED8435744C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3933,7 +4009,7 @@
         <xdr:cNvPr id="226" name="Rectangle 225">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43293255-1E5C-6D64-B6B5-4C534012B38A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{43293255-1E5C-6D64-B6B5-4C534012B38A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3996,7 +4072,7 @@
         <xdr:cNvPr id="200" name="Straight Arrow Connector 199">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6742F96-6706-4F25-2402-16D113F50115}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A6742F96-6706-4F25-2402-16D113F50115}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4052,7 +4128,7 @@
         <xdr:cNvPr id="203" name="Connector: Elbow 202">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C05F93F-4491-1089-9C75-95522BE2D55F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3C05F93F-4491-1089-9C75-95522BE2D55F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4108,7 +4184,7 @@
         <xdr:cNvPr id="204" name="Rectangle 203">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CC39AC3-D31A-3DEB-3FA3-30B6E9970945}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2CC39AC3-D31A-3DEB-3FA3-30B6E9970945}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4178,7 +4254,7 @@
         <xdr:cNvPr id="277" name="Rectangle 276">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9756E1D-6F8D-1F73-125B-283F0DE30E65}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A9756E1D-6F8D-1F73-125B-283F0DE30E65}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4262,7 +4338,7 @@
         <xdr:cNvPr id="291" name="Rectangle 290">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF98E191-C7E4-E3CC-8C70-430CA3D8877C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BF98E191-C7E4-E3CC-8C70-430CA3D8877C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4325,7 +4401,7 @@
         <xdr:cNvPr id="293" name="Rectangle 292">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A0868AF-0480-E151-77F7-48BBCAD87EBE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4A0868AF-0480-E151-77F7-48BBCAD87EBE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4393,7 +4469,7 @@
         <xdr:cNvPr id="300" name="Rectangle 299">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E6E3BFD-0229-1CE5-EE43-A63860D12EBE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6E6E3BFD-0229-1CE5-EE43-A63860D12EBE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4475,7 +4551,7 @@
         <xdr:cNvPr id="301" name="Rectangle 300">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DCF44B1-E01B-8F32-6664-957E27134710}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8DCF44B1-E01B-8F32-6664-957E27134710}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4550,7 +4626,7 @@
         <xdr:cNvPr id="302" name="Rectangle 301">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D146A799-3F91-BEA2-C4AC-70D0BFB81705}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D146A799-3F91-BEA2-C4AC-70D0BFB81705}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4620,7 +4696,7 @@
         <xdr:cNvPr id="303" name="Rectangle 302">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D11C16C0-C18D-908F-0C8F-19BD003ADB1A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D11C16C0-C18D-908F-0C8F-19BD003ADB1A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4712,7 +4788,7 @@
         <xdr:cNvPr id="304" name="Rectangle 303">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38825BBC-E7DA-8E56-346A-DDBBD3BFB779}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{38825BBC-E7DA-8E56-346A-DDBBD3BFB779}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4860,7 +4936,7 @@
         <xdr:cNvPr id="237" name="Straight Arrow Connector 236">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{037BC34B-6C53-3788-40A5-DAC45ED79BB9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{037BC34B-6C53-3788-40A5-DAC45ED79BB9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4916,7 +4992,7 @@
         <xdr:cNvPr id="239" name="Straight Arrow Connector 238">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CE8FD69-B553-CCDC-31AA-09D8966076F0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7CE8FD69-B553-CCDC-31AA-09D8966076F0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4972,7 +5048,7 @@
         <xdr:cNvPr id="241" name="Straight Arrow Connector 240">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1C676F3-8BEF-A082-3DD6-F6AD8E75064A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E1C676F3-8BEF-A082-3DD6-F6AD8E75064A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5028,7 +5104,7 @@
         <xdr:cNvPr id="245" name="Straight Arrow Connector 244">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1D134DC-5B05-FA17-30E8-2C3E2062CA13}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C1D134DC-5B05-FA17-30E8-2C3E2062CA13}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5084,7 +5160,7 @@
         <xdr:cNvPr id="247" name="Straight Arrow Connector 246">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00161F50-D4EE-ED6B-BC73-FCE6E53DAA69}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00161F50-D4EE-ED6B-BC73-FCE6E53DAA69}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5140,7 +5216,7 @@
         <xdr:cNvPr id="249" name="Straight Arrow Connector 248">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A9250D8-1B9A-5DF4-B5F1-5B12D556DAE9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5A9250D8-1B9A-5DF4-B5F1-5B12D556DAE9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5196,7 +5272,7 @@
         <xdr:cNvPr id="252" name="Straight Arrow Connector 251">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F22E0AB-0901-8AF5-3AF6-5531E8346140}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4F22E0AB-0901-8AF5-3AF6-5531E8346140}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5252,7 +5328,7 @@
         <xdr:cNvPr id="344" name="Rectangle 343">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15C556D5-CFE2-5B92-F0B7-618EA2C8C2C3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{15C556D5-CFE2-5B92-F0B7-618EA2C8C2C3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5315,7 +5391,7 @@
         <xdr:cNvPr id="272" name="Straight Arrow Connector 271">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D3A92E1-E68B-2036-35C8-C08772D9A190}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7D3A92E1-E68B-2036-35C8-C08772D9A190}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5371,7 +5447,7 @@
         <xdr:cNvPr id="348" name="Rectangle 347">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B4943A5-87A8-8961-F71B-CF985DA7737F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4B4943A5-87A8-8961-F71B-CF985DA7737F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5434,7 +5510,7 @@
         <xdr:cNvPr id="349" name="Rectangle 348">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE70EF5F-57EE-538D-1A2B-6CE761C2A3EC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AE70EF5F-57EE-538D-1A2B-6CE761C2A3EC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5497,7 +5573,7 @@
         <xdr:cNvPr id="350" name="Rectangle 349">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FD6BAA2-6530-2210-8E3E-BEE408084FE2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5FD6BAA2-6530-2210-8E3E-BEE408084FE2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5565,7 +5641,7 @@
         <xdr:cNvPr id="353" name="Rectangle 352">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0CF8AB2-E6DF-7400-C8D1-D71662BA4395}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0CF8AB2-E6DF-7400-C8D1-D71662BA4395}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5628,7 +5704,7 @@
         <xdr:cNvPr id="354" name="Rectangle 353">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC19F654-D768-AED9-5333-191F663C8E48}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EC19F654-D768-AED9-5333-191F663C8E48}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5691,7 +5767,7 @@
         <xdr:cNvPr id="275" name="Connector: Elbow 274">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C9492A7-0C08-175E-FBA6-2D5CB2631358}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9C9492A7-0C08-175E-FBA6-2D5CB2631358}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5747,7 +5823,7 @@
         <xdr:cNvPr id="284" name="Connector: Elbow 283">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7FE5FB1-3A1D-BE07-BD5E-E9417CD08CAA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E7FE5FB1-3A1D-BE07-BD5E-E9417CD08CAA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5803,7 +5879,7 @@
         <xdr:cNvPr id="286" name="Connector: Elbow 285">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F891C8B-0021-74DF-749D-0D7841441398}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1F891C8B-0021-74DF-749D-0D7841441398}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5859,7 +5935,7 @@
         <xdr:cNvPr id="288" name="Connector: Elbow 287">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1F9DDA5-4B78-477C-6C18-243D1EF4BFDE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A1F9DDA5-4B78-477C-6C18-243D1EF4BFDE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5915,7 +5991,7 @@
         <xdr:cNvPr id="290" name="Connector: Elbow 289">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1666855-92A2-6E3D-DDEC-4E081B1D4307}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E1666855-92A2-6E3D-DDEC-4E081B1D4307}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5971,7 +6047,7 @@
         <xdr:cNvPr id="297" name="Connector: Elbow 296">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95F949F4-0904-BFEA-9154-26FFBB4FA87F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{95F949F4-0904-BFEA-9154-26FFBB4FA87F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6027,7 +6103,7 @@
         <xdr:cNvPr id="299" name="Connector: Elbow 298">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A9E6B12-2431-00DD-AA78-5479B0E4A645}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1A9E6B12-2431-00DD-AA78-5479B0E4A645}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6083,7 +6159,7 @@
         <xdr:cNvPr id="306" name="Connector: Elbow 305">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F167EA2F-C46A-908F-16D9-5A97EE7CC6BD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F167EA2F-C46A-908F-16D9-5A97EE7CC6BD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6139,7 +6215,7 @@
         <xdr:cNvPr id="308" name="Connector: Elbow 307">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B93CA3EE-65C6-1DA7-3F20-981F04EED772}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B93CA3EE-65C6-1DA7-3F20-981F04EED772}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6195,7 +6271,7 @@
         <xdr:cNvPr id="310" name="Connector: Elbow 309">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0B05704-F543-2E75-7D0D-FCDD5E4C8C86}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F0B05704-F543-2E75-7D0D-FCDD5E4C8C86}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6251,7 +6327,7 @@
         <xdr:cNvPr id="312" name="Straight Arrow Connector 311">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A0AABE3-E6BB-B42F-95EA-D67EE8E5D378}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7A0AABE3-E6BB-B42F-95EA-D67EE8E5D378}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6307,7 +6383,7 @@
         <xdr:cNvPr id="320" name="Straight Arrow Connector 319">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90354B19-6855-E0D8-680D-1E4105DF0482}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{90354B19-6855-E0D8-680D-1E4105DF0482}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6363,7 +6439,7 @@
         <xdr:cNvPr id="322" name="Rectangle 321">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A18F4F7C-87F5-DB03-151D-A83CCBEC56DA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A18F4F7C-87F5-DB03-151D-A83CCBEC56DA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6426,7 +6502,7 @@
         <xdr:cNvPr id="395" name="Rectangle 394">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EBD1FD7-007B-D887-47BA-DA775FEB2509}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8EBD1FD7-007B-D887-47BA-DA775FEB2509}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6489,7 +6565,7 @@
         <xdr:cNvPr id="396" name="Rectangle 395">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83417375-8D54-3374-22BD-906DEC74C681}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{83417375-8D54-3374-22BD-906DEC74C681}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6552,7 +6628,7 @@
         <xdr:cNvPr id="399" name="Rectangle 398">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7EBE78C-9D75-0F1B-994D-E45226229227}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F7EBE78C-9D75-0F1B-994D-E45226229227}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6620,7 +6696,7 @@
         <xdr:cNvPr id="402" name="Rectangle 401">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBFF531B-51DB-1F6D-EB96-AD7CC80D0F67}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BBFF531B-51DB-1F6D-EB96-AD7CC80D0F67}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6688,7 +6764,7 @@
         <xdr:cNvPr id="403" name="Rectangle 402">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C54CE03-4CBF-AB6C-446A-DFE119647AF5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8C54CE03-4CBF-AB6C-446A-DFE119647AF5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6756,7 +6832,7 @@
         <xdr:cNvPr id="324" name="Connector: Elbow 323">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B3106B3-9F5E-2D68-A93F-EAD98281AF68}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6B3106B3-9F5E-2D68-A93F-EAD98281AF68}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6814,7 +6890,7 @@
         <xdr:cNvPr id="326" name="Connector: Elbow 325">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A5A3CC7-F5E3-3A59-AAE6-5A77EF8AF76B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7A5A3CC7-F5E3-3A59-AAE6-5A77EF8AF76B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6872,7 +6948,7 @@
         <xdr:cNvPr id="328" name="Connector: Elbow 327">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59EA8637-5020-E5F2-74D2-94F1EF7FC222}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{59EA8637-5020-E5F2-74D2-94F1EF7FC222}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6930,7 +7006,7 @@
         <xdr:cNvPr id="330" name="Straight Arrow Connector 329">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B02CCDB-FA0B-72B0-A09C-FD22650E550C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2B02CCDB-FA0B-72B0-A09C-FD22650E550C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6986,7 +7062,7 @@
         <xdr:cNvPr id="333" name="Straight Arrow Connector 332">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A3EDF1A-1180-3DE2-F794-2034477DD130}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5A3EDF1A-1180-3DE2-F794-2034477DD130}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7042,7 +7118,7 @@
         <xdr:cNvPr id="336" name="Straight Arrow Connector 335">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D49E3D0B-1038-9898-7459-1899641E9168}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D49E3D0B-1038-9898-7459-1899641E9168}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7098,7 +7174,7 @@
         <xdr:cNvPr id="337" name="Diamond 336">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BEFA8B7-6CAC-A993-6CF5-2F9AE9E84215}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0BEFA8B7-6CAC-A993-6CF5-2F9AE9E84215}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7161,7 +7237,7 @@
         <xdr:cNvPr id="339" name="Straight Arrow Connector 338">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{031A5C72-A1A6-5D91-E183-A0A5BB5F4281}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{031A5C72-A1A6-5D91-E183-A0A5BB5F4281}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7217,7 +7293,7 @@
         <xdr:cNvPr id="345" name="Connector: Elbow 344">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1A60F90-7E17-D5BC-885D-93CF3719F5E5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E1A60F90-7E17-D5BC-885D-93CF3719F5E5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7273,7 +7349,7 @@
         <xdr:cNvPr id="357" name="Rectangle 356">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D4713C5-EDD9-4EA1-A109-F2489A23AA03}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5D4713C5-EDD9-4EA1-A109-F2489A23AA03}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7336,7 +7412,7 @@
         <xdr:cNvPr id="359" name="Straight Arrow Connector 358">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB0E2081-9AA7-67A9-D00B-7B6185BDEF36}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AB0E2081-9AA7-67A9-D00B-7B6185BDEF36}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7392,7 +7468,7 @@
         <xdr:cNvPr id="434" name="Rectangle 433">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{141C32BC-CF88-A0F0-A5FF-F2D39ECEE99A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{141C32BC-CF88-A0F0-A5FF-F2D39ECEE99A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7455,7 +7531,7 @@
         <xdr:cNvPr id="364" name="Connector: Elbow 363">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12FAF3DF-F9A7-21C4-6847-2432DF2AA5E8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{12FAF3DF-F9A7-21C4-6847-2432DF2AA5E8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7511,7 +7587,7 @@
         <xdr:cNvPr id="369" name="Straight Arrow Connector 368">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BA1F722-0166-8592-56C3-87D42892EE44}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0BA1F722-0166-8592-56C3-87D42892EE44}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7568,7 +7644,7 @@
         <xdr:cNvPr id="450" name="Rectangle 449">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{886D6DE6-1F36-FDA4-7903-597ECC919057}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{886D6DE6-1F36-FDA4-7903-597ECC919057}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7631,7 +7707,7 @@
         <xdr:cNvPr id="376" name="Straight Arrow Connector 375">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{064EF7AD-9F40-2DE8-EA0E-A5AD3E1983B5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{064EF7AD-9F40-2DE8-EA0E-A5AD3E1983B5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7688,7 +7764,7 @@
         <xdr:cNvPr id="464" name="Diamond 463">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C915F7B-BCE8-F060-1A20-20EB22B6006C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1C915F7B-BCE8-F060-1A20-20EB22B6006C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7759,7 +7835,7 @@
         <xdr:cNvPr id="454" name="Straight Arrow Connector 453">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E42FBB5-4535-71B8-FC68-8C7AFD6E4B7F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1E42FBB5-4535-71B8-FC68-8C7AFD6E4B7F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7816,7 +7892,7 @@
         <xdr:cNvPr id="461" name="Connector: Elbow 460">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E7714BA-E693-0D0A-6072-A8E598E8295E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4E7714BA-E693-0D0A-6072-A8E598E8295E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7872,7 +7948,7 @@
         <xdr:cNvPr id="478" name="Rectangle 477">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0212693D-D747-7775-BC2D-3520099979DA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0212693D-D747-7775-BC2D-3520099979DA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7935,7 +8011,7 @@
         <xdr:cNvPr id="482" name="Rectangle 481">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75D29002-7C66-2BC2-B0F6-DD3D754C32C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{75D29002-7C66-2BC2-B0F6-DD3D754C32C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7998,7 +8074,7 @@
         <xdr:cNvPr id="492" name="Rectangle 491">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41052F66-A624-F367-37B3-99FE9D72B420}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{41052F66-A624-F367-37B3-99FE9D72B420}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8061,7 +8137,7 @@
         <xdr:cNvPr id="481" name="Connector: Elbow 480">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A573981-F25B-1098-D017-0236FFF65BE8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7A573981-F25B-1098-D017-0236FFF65BE8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8117,7 +8193,7 @@
         <xdr:cNvPr id="488" name="Connector: Elbow 487">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49A0DB27-929E-5664-DD03-81AA2115F925}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{49A0DB27-929E-5664-DD03-81AA2115F925}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8173,7 +8249,7 @@
         <xdr:cNvPr id="503" name="Rectangle 502">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{634D115F-BA9D-AC73-8DC5-B177DA0DD039}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{634D115F-BA9D-AC73-8DC5-B177DA0DD039}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8236,7 +8312,7 @@
         <xdr:cNvPr id="504" name="Rectangle 503">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C8AF2C4-7266-FDA9-FE08-9BC163C40C03}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4C8AF2C4-7266-FDA9-FE08-9BC163C40C03}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8299,7 +8375,7 @@
         <xdr:cNvPr id="506" name="Rectangle 505">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2EBDBA8-B02C-6E11-A5CF-FA19199D9839}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B2EBDBA8-B02C-6E11-A5CF-FA19199D9839}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8362,7 +8438,7 @@
         <xdr:cNvPr id="493" name="Straight Arrow Connector 492">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C5F366E-B404-0BA8-F762-9F87E334EC57}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1C5F366E-B404-0BA8-F762-9F87E334EC57}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8418,7 +8494,7 @@
         <xdr:cNvPr id="496" name="Connector: Elbow 495">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A80C5828-9CA4-C951-9EC9-5C2405DB08ED}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A80C5828-9CA4-C951-9EC9-5C2405DB08ED}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8477,7 +8553,7 @@
         <xdr:cNvPr id="500" name="Connector: Elbow 499">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA55F324-FAA1-95C5-EDBB-B4F5BBF0B7B7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DA55F324-FAA1-95C5-EDBB-B4F5BBF0B7B7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8536,7 +8612,7 @@
         <xdr:cNvPr id="511" name="Connector: Elbow 510">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB2BDA04-D53F-E16F-40A1-938A443CB78D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FB2BDA04-D53F-E16F-40A1-938A443CB78D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8594,7 +8670,7 @@
         <xdr:cNvPr id="386" name="Connector: Elbow 385">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA2EA158-DD4C-9291-BFDE-414B28197C4B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EA2EA158-DD4C-9291-BFDE-414B28197C4B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8652,7 +8728,7 @@
         <xdr:cNvPr id="389" name="Connector: Elbow 388">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04FCD762-69B4-BDC9-5296-2856FFD8E380}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{04FCD762-69B4-BDC9-5296-2856FFD8E380}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8710,7 +8786,7 @@
         <xdr:cNvPr id="412" name="Straight Arrow Connector 411">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{214C2CBF-3AAB-DD40-58CA-B954AB2B953A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{214C2CBF-3AAB-DD40-58CA-B954AB2B953A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8766,7 +8842,7 @@
         <xdr:cNvPr id="549" name="Rectangle 548">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60EC7015-674F-C035-8A3D-90110260656A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{60EC7015-674F-C035-8A3D-90110260656A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8834,7 +8910,7 @@
         <xdr:cNvPr id="416" name="Connector: Elbow 415">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED0A8ADD-472B-E68A-3C0B-16A5345DF3E6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{ED0A8ADD-472B-E68A-3C0B-16A5345DF3E6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8890,7 +8966,7 @@
         <xdr:cNvPr id="557" name="Rectangle 556">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39EE8E70-69CA-73EB-081F-BFD537140F70}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{39EE8E70-69CA-73EB-081F-BFD537140F70}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8953,7 +9029,7 @@
         <xdr:cNvPr id="558" name="Rectangle 557">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30CE8806-D8D3-043E-346A-A936E52B704A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{30CE8806-D8D3-043E-346A-A936E52B704A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9016,7 +9092,7 @@
         <xdr:cNvPr id="559" name="Rectangle 558">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{234B76E3-C775-CB01-C51C-AE1B4C69027E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{234B76E3-C775-CB01-C51C-AE1B4C69027E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9084,7 +9160,7 @@
         <xdr:cNvPr id="560" name="Rectangle 559">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{472B8B14-8E1B-9E34-134D-077077E66926}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{472B8B14-8E1B-9E34-134D-077077E66926}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9147,7 +9223,7 @@
         <xdr:cNvPr id="561" name="Rectangle 560">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18A97039-056A-1BD6-2301-C7BB59A76C0F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{18A97039-056A-1BD6-2301-C7BB59A76C0F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9215,7 +9291,7 @@
         <xdr:cNvPr id="571" name="Rectangle 570">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E953785-7D8E-4AB8-5E1E-FA2F76927701}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5E953785-7D8E-4AB8-5E1E-FA2F76927701}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9283,7 +9359,7 @@
         <xdr:cNvPr id="429" name="Straight Arrow Connector 428">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CED1465-A771-205C-BBB6-126543509F4D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9CED1465-A771-205C-BBB6-126543509F4D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9339,7 +9415,7 @@
         <xdr:cNvPr id="431" name="Connector: Elbow 430">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{150A048A-D91E-76D5-513B-C8368E72C1B2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{150A048A-D91E-76D5-513B-C8368E72C1B2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9394,7 +9470,7 @@
         <xdr:cNvPr id="441" name="Connector: Elbow 440">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92A6C576-189D-57D5-C549-754EC4BF4FFB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{92A6C576-189D-57D5-C549-754EC4BF4FFB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9450,7 +9526,7 @@
         <xdr:cNvPr id="444" name="Connector: Elbow 443">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA5BD2F3-5151-9F42-96B2-B89822A7CB02}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BA5BD2F3-5151-9F42-96B2-B89822A7CB02}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9506,7 +9582,7 @@
         <xdr:cNvPr id="447" name="Straight Arrow Connector 446">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EA4DAB3-9587-14ED-27A9-B222D0C3BEE3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4EA4DAB3-9587-14ED-27A9-B222D0C3BEE3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9562,7 +9638,7 @@
         <xdr:cNvPr id="603" name="Rectangle 602">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A717D765-1050-685D-E446-A48827097EFD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A717D765-1050-685D-E446-A48827097EFD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9626,7 +9702,7 @@
         <xdr:cNvPr id="526" name="Connector: Elbow 525">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CCBB9D3-5B46-9C7E-1526-94F5B3F7D2E7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7CCBB9D3-5B46-9C7E-1526-94F5B3F7D2E7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9682,7 +9758,7 @@
         <xdr:cNvPr id="536" name="Connector: Elbow 535">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09CA61CF-1388-18BE-2EF6-C3AE83632FFA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{09CA61CF-1388-18BE-2EF6-C3AE83632FFA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9738,7 +9814,7 @@
         <xdr:cNvPr id="542" name="Connector: Elbow 541">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DB857A0-7AEE-F980-E064-1A06168B078B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9DB857A0-7AEE-F980-E064-1A06168B078B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9798,7 +9874,7 @@
         <xdr:cNvPr id="625" name="Rectangle 624">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{833FB374-0FE6-CB77-2438-275E7FD5493B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{833FB374-0FE6-CB77-2438-275E7FD5493B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9866,7 +9942,7 @@
         <xdr:cNvPr id="627" name="Rectangle 626">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAEA01B5-FF22-DD48-20CD-315D29C37784}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BAEA01B5-FF22-DD48-20CD-315D29C37784}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9929,7 +10005,7 @@
         <xdr:cNvPr id="565" name="Connector: Elbow 564">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{328480B0-0FBA-11FA-3C67-15DB6636684A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{328480B0-0FBA-11FA-3C67-15DB6636684A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9988,7 +10064,7 @@
         <xdr:cNvPr id="117" name="Rectangle 116">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{985192AB-8642-07F8-E04D-8EBAD661EEAF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{985192AB-8642-07F8-E04D-8EBAD661EEAF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10051,7 +10127,7 @@
         <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78333CFC-7F9C-DFFD-6398-476B4710F7FA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{78333CFC-7F9C-DFFD-6398-476B4710F7FA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10107,7 +10183,7 @@
         <xdr:cNvPr id="115" name="Rectangle 114">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED1F65BD-EFB7-BEFF-549F-9E4E36C12FAD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{ED1F65BD-EFB7-BEFF-549F-9E4E36C12FAD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10170,7 +10246,7 @@
         <xdr:cNvPr id="5" name="Connector: Elbow 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D31A361-7A62-F6FA-A055-24AA616A93D9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4D31A361-7A62-F6FA-A055-24AA616A93D9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10233,7 +10309,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{943D27F9-5766-34FB-9C45-9266F0C7C4EC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{943D27F9-5766-34FB-9C45-9266F0C7C4EC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10283,7 +10359,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59CF1D88-4644-4D1C-3C67-0C7C9ED14102}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{59CF1D88-4644-4D1C-3C67-0C7C9ED14102}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10333,7 +10409,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{402A2CA2-4F18-49E8-E32F-820D6D50FE9F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{402A2CA2-4F18-49E8-E32F-820D6D50FE9F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10383,7 +10459,7 @@
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{431B73F5-8533-5F90-FAC6-4715CF6D697C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{431B73F5-8533-5F90-FAC6-4715CF6D697C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10433,7 +10509,7 @@
         <xdr:cNvPr id="11" name="Picture 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F4E30CE-2ED6-2389-AB94-DE2D102A300B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3F4E30CE-2ED6-2389-AB94-DE2D102A300B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10483,7 +10559,7 @@
         <xdr:cNvPr id="13" name="Picture 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B91832F-DEB0-AB70-6808-E9D212BCA607}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2B91832F-DEB0-AB70-6808-E9D212BCA607}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10533,7 +10609,7 @@
         <xdr:cNvPr id="15" name="Picture 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{358E9180-29A8-EEBE-A22F-5CC8BD7C3822}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{358E9180-29A8-EEBE-A22F-5CC8BD7C3822}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10583,7 +10659,7 @@
         <xdr:cNvPr id="17" name="Picture 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A80411B2-C71C-C4CB-B458-75B436F160CB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A80411B2-C71C-C4CB-B458-75B436F160CB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10633,7 +10709,7 @@
         <xdr:cNvPr id="19" name="Picture 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D919F268-10D5-ED58-B6E9-080AF2265538}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D919F268-10D5-ED58-B6E9-080AF2265538}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10683,7 +10759,7 @@
         <xdr:cNvPr id="21" name="Picture 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BA4512C-EFFB-8859-8461-70AC52D3D87C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9BA4512C-EFFB-8859-8461-70AC52D3D87C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10733,7 +10809,7 @@
         <xdr:cNvPr id="23" name="Picture 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{618098A7-3E95-CD4B-7CFA-C9B2C18A71B4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{618098A7-3E95-CD4B-7CFA-C9B2C18A71B4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10783,7 +10859,7 @@
         <xdr:cNvPr id="25" name="Picture 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{277C99A9-FD84-15A8-64C2-0854E5AE8439}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{277C99A9-FD84-15A8-64C2-0854E5AE8439}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10833,7 +10909,7 @@
         <xdr:cNvPr id="27" name="Picture 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DE6154F-5721-F549-FCEA-3DCAEC4EBEA0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0DE6154F-5721-F549-FCEA-3DCAEC4EBEA0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10883,7 +10959,7 @@
         <xdr:cNvPr id="29" name="Picture 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0156D0A8-32AA-59F9-E6EB-EE2C740A875F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0156D0A8-32AA-59F9-E6EB-EE2C740A875F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10933,7 +11009,7 @@
         <xdr:cNvPr id="31" name="Picture 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CF0CE33-63CF-8316-831B-FA7C09D6B069}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9CF0CE33-63CF-8316-831B-FA7C09D6B069}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11264,10 +11340,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A32" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11564,22 +11640,22 @@
       <c r="N18" s="14"/>
     </row>
     <row r="19" spans="1:14" ht="92.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="544" t="s">
+      <c r="A19" s="547" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="545"/>
-      <c r="C19" s="545"/>
-      <c r="D19" s="545"/>
-      <c r="E19" s="545"/>
-      <c r="F19" s="545"/>
-      <c r="G19" s="545"/>
-      <c r="H19" s="545"/>
-      <c r="I19" s="545"/>
-      <c r="J19" s="545"/>
-      <c r="K19" s="545"/>
-      <c r="L19" s="545"/>
-      <c r="M19" s="545"/>
-      <c r="N19" s="546"/>
+      <c r="B19" s="548"/>
+      <c r="C19" s="548"/>
+      <c r="D19" s="548"/>
+      <c r="E19" s="548"/>
+      <c r="F19" s="548"/>
+      <c r="G19" s="548"/>
+      <c r="H19" s="548"/>
+      <c r="I19" s="548"/>
+      <c r="J19" s="548"/>
+      <c r="K19" s="548"/>
+      <c r="L19" s="548"/>
+      <c r="M19" s="548"/>
+      <c r="N19" s="549"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
@@ -11614,22 +11690,22 @@
       <c r="N21" s="14"/>
     </row>
     <row r="22" spans="1:14" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="A22" s="541" t="s">
+      <c r="A22" s="544" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="542"/>
-      <c r="C22" s="542"/>
-      <c r="D22" s="542"/>
-      <c r="E22" s="542"/>
-      <c r="F22" s="542"/>
-      <c r="G22" s="542"/>
-      <c r="H22" s="542"/>
-      <c r="I22" s="542"/>
-      <c r="J22" s="542"/>
-      <c r="K22" s="542"/>
-      <c r="L22" s="542"/>
-      <c r="M22" s="542"/>
-      <c r="N22" s="543"/>
+      <c r="B22" s="545"/>
+      <c r="C22" s="545"/>
+      <c r="D22" s="545"/>
+      <c r="E22" s="545"/>
+      <c r="F22" s="545"/>
+      <c r="G22" s="545"/>
+      <c r="H22" s="545"/>
+      <c r="I22" s="545"/>
+      <c r="J22" s="545"/>
+      <c r="K22" s="545"/>
+      <c r="L22" s="545"/>
+      <c r="M22" s="545"/>
+      <c r="N22" s="546"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
@@ -11937,10 +12013,10 @@
     </row>
     <row r="42" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A42" s="13"/>
-      <c r="B42" s="539" t="s">
+      <c r="B42" s="542" t="s">
         <v>19</v>
       </c>
-      <c r="C42" s="539"/>
+      <c r="C42" s="542"/>
       <c r="D42" s="20">
         <v>1</v>
       </c>
@@ -12064,13 +12140,13 @@
       <c r="H48" s="6"/>
       <c r="I48" s="6"/>
       <c r="J48" s="6"/>
-      <c r="K48" s="540" t="s">
+      <c r="K48" s="543" t="s">
         <v>21</v>
       </c>
-      <c r="L48" s="540"/>
+      <c r="L48" s="543"/>
       <c r="M48" s="19">
         <f ca="1">NOW()</f>
-        <v>44706.97908344907</v>
+        <v>44707.943716203707</v>
       </c>
       <c r="N48" s="14"/>
     </row>
@@ -12085,13 +12161,13 @@
       <c r="H49" s="6"/>
       <c r="I49" s="6"/>
       <c r="J49" s="6"/>
-      <c r="K49" s="540" t="s">
+      <c r="K49" s="543" t="s">
         <v>20</v>
       </c>
-      <c r="L49" s="540"/>
+      <c r="L49" s="543"/>
       <c r="M49" s="19">
         <f ca="1">NOW()</f>
-        <v>44706.97908344907</v>
+        <v>44707.943716203707</v>
       </c>
       <c r="N49" s="14"/>
     </row>
@@ -12141,7 +12217,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q70"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
@@ -12154,54 +12230,54 @@
   <sheetData>
     <row r="1" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:17" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="547" t="s">
+      <c r="A2" s="550" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="548"/>
-      <c r="C2" s="551" t="s">
+      <c r="B2" s="551"/>
+      <c r="C2" s="554" t="s">
         <v>119</v>
       </c>
-      <c r="D2" s="552"/>
-      <c r="E2" s="552"/>
-      <c r="F2" s="552"/>
-      <c r="G2" s="552"/>
-      <c r="H2" s="552"/>
-      <c r="I2" s="552"/>
-      <c r="J2" s="552"/>
-      <c r="K2" s="552"/>
-      <c r="L2" s="552"/>
-      <c r="M2" s="552"/>
-      <c r="N2" s="552"/>
+      <c r="D2" s="555"/>
+      <c r="E2" s="555"/>
+      <c r="F2" s="555"/>
+      <c r="G2" s="555"/>
+      <c r="H2" s="555"/>
+      <c r="I2" s="555"/>
+      <c r="J2" s="555"/>
+      <c r="K2" s="555"/>
+      <c r="L2" s="555"/>
+      <c r="M2" s="555"/>
+      <c r="N2" s="555"/>
       <c r="O2" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="P2" s="555">
+      <c r="P2" s="558">
         <v>44698</v>
       </c>
-      <c r="Q2" s="556"/>
+      <c r="Q2" s="559"/>
     </row>
     <row r="3" spans="1:17" ht="33.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="549"/>
-      <c r="B3" s="550"/>
-      <c r="C3" s="553"/>
-      <c r="D3" s="554"/>
-      <c r="E3" s="554"/>
-      <c r="F3" s="554"/>
-      <c r="G3" s="554"/>
-      <c r="H3" s="554"/>
-      <c r="I3" s="554"/>
-      <c r="J3" s="554"/>
-      <c r="K3" s="554"/>
-      <c r="L3" s="554"/>
-      <c r="M3" s="554"/>
-      <c r="N3" s="554"/>
+      <c r="A3" s="552"/>
+      <c r="B3" s="553"/>
+      <c r="C3" s="556"/>
+      <c r="D3" s="557"/>
+      <c r="E3" s="557"/>
+      <c r="F3" s="557"/>
+      <c r="G3" s="557"/>
+      <c r="H3" s="557"/>
+      <c r="I3" s="557"/>
+      <c r="J3" s="557"/>
+      <c r="K3" s="557"/>
+      <c r="L3" s="557"/>
+      <c r="M3" s="557"/>
+      <c r="N3" s="557"/>
       <c r="O3" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="557">
+      <c r="P3" s="560">
         <v>44698</v>
       </c>
-      <c r="Q3" s="558"/>
+      <c r="Q3" s="561"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
@@ -13240,10 +13316,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O116"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="140" zoomScaleSheetLayoutView="70" workbookViewId="0"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="140" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13260,50 +13336,50 @@
   <sheetData>
     <row r="1" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:15" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="547" t="s">
+      <c r="A2" s="550" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="548"/>
-      <c r="C2" s="551" t="s">
+      <c r="B2" s="551"/>
+      <c r="C2" s="554" t="s">
         <v>119</v>
       </c>
-      <c r="D2" s="552"/>
-      <c r="E2" s="552"/>
-      <c r="F2" s="552"/>
-      <c r="G2" s="552"/>
-      <c r="H2" s="552"/>
-      <c r="I2" s="552"/>
-      <c r="J2" s="552"/>
-      <c r="K2" s="552"/>
-      <c r="L2" s="552"/>
+      <c r="D2" s="555"/>
+      <c r="E2" s="555"/>
+      <c r="F2" s="555"/>
+      <c r="G2" s="555"/>
+      <c r="H2" s="555"/>
+      <c r="I2" s="555"/>
+      <c r="J2" s="555"/>
+      <c r="K2" s="555"/>
+      <c r="L2" s="555"/>
       <c r="M2" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="555">
+      <c r="N2" s="558">
         <v>44698</v>
       </c>
-      <c r="O2" s="556"/>
+      <c r="O2" s="559"/>
     </row>
     <row r="3" spans="1:15" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="549"/>
-      <c r="B3" s="550"/>
-      <c r="C3" s="553"/>
-      <c r="D3" s="554"/>
-      <c r="E3" s="554"/>
-      <c r="F3" s="554"/>
-      <c r="G3" s="554"/>
-      <c r="H3" s="554"/>
-      <c r="I3" s="554"/>
-      <c r="J3" s="554"/>
-      <c r="K3" s="554"/>
-      <c r="L3" s="554"/>
+      <c r="A3" s="552"/>
+      <c r="B3" s="553"/>
+      <c r="C3" s="556"/>
+      <c r="D3" s="557"/>
+      <c r="E3" s="557"/>
+      <c r="F3" s="557"/>
+      <c r="G3" s="557"/>
+      <c r="H3" s="557"/>
+      <c r="I3" s="557"/>
+      <c r="J3" s="557"/>
+      <c r="K3" s="557"/>
+      <c r="L3" s="557"/>
       <c r="M3" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="N3" s="557">
+      <c r="N3" s="560">
         <v>44698</v>
       </c>
-      <c r="O3" s="558"/>
+      <c r="O3" s="561"/>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
@@ -16723,7 +16799,469 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U20"/>
+  <sheetViews>
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="140" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5" style="412" customWidth="1"/>
+    <col min="2" max="2" width="16.375" style="412" customWidth="1"/>
+    <col min="3" max="3" width="6.875" style="412" customWidth="1"/>
+    <col min="4" max="4" width="7" style="412" customWidth="1"/>
+    <col min="5" max="5" width="6.75" style="412" customWidth="1"/>
+    <col min="6" max="6" width="6.875" style="412" customWidth="1"/>
+    <col min="7" max="7" width="6.125" style="412" customWidth="1"/>
+    <col min="8" max="13" width="6.75" style="412" customWidth="1"/>
+    <col min="14" max="17" width="7.5" style="412" customWidth="1"/>
+    <col min="18" max="19" width="8" style="412" customWidth="1"/>
+    <col min="20" max="20" width="5.625" style="412" customWidth="1"/>
+    <col min="21" max="16384" width="11" style="412"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:21" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="550" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="551"/>
+      <c r="C2" s="555"/>
+      <c r="D2" s="555"/>
+      <c r="E2" s="555"/>
+      <c r="F2" s="555"/>
+      <c r="G2" s="555"/>
+      <c r="H2" s="555"/>
+      <c r="I2" s="555"/>
+      <c r="J2" s="555"/>
+      <c r="K2" s="555"/>
+      <c r="L2" s="555"/>
+      <c r="M2" s="555"/>
+      <c r="N2" s="555"/>
+      <c r="O2" s="555"/>
+      <c r="P2" s="555"/>
+      <c r="Q2" s="555"/>
+      <c r="R2" s="555"/>
+      <c r="S2" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="T2" s="558">
+        <v>44698</v>
+      </c>
+      <c r="U2" s="559"/>
+    </row>
+    <row r="3" spans="1:21" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="552"/>
+      <c r="B3" s="553"/>
+      <c r="C3" s="557"/>
+      <c r="D3" s="557"/>
+      <c r="E3" s="557"/>
+      <c r="F3" s="557"/>
+      <c r="G3" s="557"/>
+      <c r="H3" s="557"/>
+      <c r="I3" s="557"/>
+      <c r="J3" s="557"/>
+      <c r="K3" s="557"/>
+      <c r="L3" s="557"/>
+      <c r="M3" s="557"/>
+      <c r="N3" s="557"/>
+      <c r="O3" s="557"/>
+      <c r="P3" s="557"/>
+      <c r="Q3" s="557"/>
+      <c r="R3" s="557"/>
+      <c r="S3" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="T3" s="560">
+        <v>44698</v>
+      </c>
+      <c r="U3" s="561"/>
+    </row>
+    <row r="4" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:21" ht="21" x14ac:dyDescent="0.35">
+      <c r="A5" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="579" t="s">
+        <v>377</v>
+      </c>
+      <c r="C5" s="42">
+        <v>17</v>
+      </c>
+      <c r="D5" s="579">
+        <v>18</v>
+      </c>
+      <c r="E5" s="579">
+        <v>19</v>
+      </c>
+      <c r="F5" s="579">
+        <v>20</v>
+      </c>
+      <c r="G5" s="579">
+        <v>21</v>
+      </c>
+      <c r="H5" s="579">
+        <v>22</v>
+      </c>
+      <c r="I5" s="579">
+        <v>23</v>
+      </c>
+      <c r="J5" s="579">
+        <v>24</v>
+      </c>
+      <c r="K5" s="579">
+        <v>25</v>
+      </c>
+      <c r="L5" s="579">
+        <v>26</v>
+      </c>
+      <c r="M5" s="579">
+        <v>27</v>
+      </c>
+      <c r="N5" s="579">
+        <v>28</v>
+      </c>
+      <c r="O5" s="579">
+        <v>29</v>
+      </c>
+      <c r="P5" s="579">
+        <v>30</v>
+      </c>
+      <c r="Q5" s="579">
+        <v>31</v>
+      </c>
+      <c r="R5" s="579">
+        <v>1</v>
+      </c>
+      <c r="S5" s="579">
+        <v>2</v>
+      </c>
+      <c r="T5" s="580">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="21" x14ac:dyDescent="0.35">
+      <c r="A6" s="44">
+        <v>1</v>
+      </c>
+      <c r="B6" s="582" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="596" t="s">
+        <v>381</v>
+      </c>
+      <c r="D6" s="595"/>
+      <c r="E6" s="595"/>
+      <c r="F6" s="595"/>
+      <c r="G6" s="595"/>
+      <c r="H6" s="597"/>
+      <c r="I6" s="578"/>
+      <c r="J6" s="578"/>
+      <c r="K6" s="578"/>
+      <c r="L6" s="578"/>
+      <c r="M6" s="578"/>
+      <c r="N6" s="48"/>
+      <c r="O6" s="48"/>
+      <c r="P6" s="48"/>
+      <c r="Q6" s="48"/>
+      <c r="R6" s="586"/>
+      <c r="S6" s="586"/>
+      <c r="T6" s="586"/>
+    </row>
+    <row r="7" spans="1:21" ht="21" x14ac:dyDescent="0.35">
+      <c r="A7" s="44">
+        <v>2</v>
+      </c>
+      <c r="B7" s="582" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="596" t="s">
+        <v>381</v>
+      </c>
+      <c r="D7" s="595"/>
+      <c r="E7" s="595"/>
+      <c r="F7" s="595"/>
+      <c r="G7" s="595"/>
+      <c r="H7" s="597"/>
+      <c r="I7" s="578"/>
+      <c r="J7" s="578"/>
+      <c r="K7" s="578"/>
+      <c r="L7" s="578"/>
+      <c r="M7" s="578"/>
+      <c r="N7" s="48"/>
+      <c r="O7" s="48"/>
+      <c r="P7" s="48"/>
+      <c r="Q7" s="48"/>
+      <c r="R7" s="586"/>
+      <c r="S7" s="586"/>
+      <c r="T7" s="586"/>
+    </row>
+    <row r="8" spans="1:21" ht="21" x14ac:dyDescent="0.35">
+      <c r="A8" s="44">
+        <v>3</v>
+      </c>
+      <c r="B8" s="582" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="590" t="s">
+        <v>379</v>
+      </c>
+      <c r="D8" s="594"/>
+      <c r="E8" s="595" t="s">
+        <v>381</v>
+      </c>
+      <c r="F8" s="592"/>
+      <c r="G8" s="592"/>
+      <c r="H8" s="593"/>
+      <c r="I8" s="578"/>
+      <c r="J8" s="578"/>
+      <c r="K8" s="578"/>
+      <c r="L8" s="578"/>
+      <c r="M8" s="578"/>
+      <c r="N8" s="48"/>
+      <c r="O8" s="48"/>
+      <c r="P8" s="48"/>
+      <c r="Q8" s="48"/>
+      <c r="R8" s="586"/>
+      <c r="S8" s="586"/>
+      <c r="T8" s="586"/>
+    </row>
+    <row r="9" spans="1:21" ht="21" x14ac:dyDescent="0.35">
+      <c r="A9" s="44">
+        <v>4</v>
+      </c>
+      <c r="B9" s="582" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="591" t="s">
+        <v>381</v>
+      </c>
+      <c r="D9" s="592"/>
+      <c r="E9" s="593"/>
+      <c r="F9" s="589" t="s">
+        <v>380</v>
+      </c>
+      <c r="G9" s="587"/>
+      <c r="H9" s="587"/>
+      <c r="I9" s="588"/>
+      <c r="J9" s="600" t="s">
+        <v>382</v>
+      </c>
+      <c r="K9" s="598"/>
+      <c r="L9" s="599"/>
+      <c r="M9" s="584"/>
+      <c r="N9" s="48"/>
+      <c r="O9" s="585"/>
+      <c r="P9" s="585"/>
+      <c r="Q9" s="585"/>
+      <c r="R9" s="586"/>
+      <c r="S9" s="586"/>
+      <c r="T9" s="586"/>
+    </row>
+    <row r="10" spans="1:21" ht="21" x14ac:dyDescent="0.35">
+      <c r="A10" s="44">
+        <v>5</v>
+      </c>
+      <c r="B10" s="582" t="s">
+        <v>378</v>
+      </c>
+      <c r="C10" s="581"/>
+      <c r="D10" s="581"/>
+      <c r="E10" s="435"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="581"/>
+      <c r="H10" s="581"/>
+      <c r="I10" s="584"/>
+      <c r="J10" s="584"/>
+      <c r="K10" s="584"/>
+      <c r="L10" s="584"/>
+      <c r="M10" s="584"/>
+      <c r="N10" s="48"/>
+      <c r="O10" s="585"/>
+      <c r="P10" s="585"/>
+      <c r="Q10" s="585"/>
+      <c r="R10" s="586"/>
+      <c r="S10" s="586"/>
+      <c r="T10" s="586"/>
+    </row>
+    <row r="11" spans="1:21" ht="21" x14ac:dyDescent="0.35">
+      <c r="A11" s="583"/>
+      <c r="B11" s="582"/>
+      <c r="C11" s="581"/>
+      <c r="D11" s="581"/>
+      <c r="E11" s="435"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="581"/>
+      <c r="H11" s="581"/>
+      <c r="I11" s="584"/>
+      <c r="J11" s="584"/>
+      <c r="K11" s="584"/>
+      <c r="L11" s="584"/>
+      <c r="M11" s="584"/>
+      <c r="N11" s="48"/>
+      <c r="O11" s="585"/>
+      <c r="P11" s="585"/>
+      <c r="Q11" s="585"/>
+      <c r="R11" s="586"/>
+      <c r="S11" s="586"/>
+      <c r="T11" s="586"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+    </row>
+    <row r="17" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+    </row>
+    <row r="18" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+    </row>
+    <row r="19" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+    </row>
+    <row r="20" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="C2:R3"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:H8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="40" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X82"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
@@ -16738,68 +17276,68 @@
   <sheetData>
     <row r="1" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:24" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="547" t="s">
+      <c r="A2" s="550" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="548"/>
-      <c r="C2" s="551" t="s">
+      <c r="B2" s="551"/>
+      <c r="C2" s="554" t="s">
         <v>119</v>
       </c>
-      <c r="D2" s="552"/>
-      <c r="E2" s="552"/>
-      <c r="F2" s="552"/>
-      <c r="G2" s="552"/>
-      <c r="H2" s="552"/>
-      <c r="I2" s="552"/>
-      <c r="J2" s="552"/>
-      <c r="K2" s="552"/>
-      <c r="L2" s="552"/>
-      <c r="M2" s="552"/>
-      <c r="N2" s="552"/>
-      <c r="O2" s="552"/>
-      <c r="P2" s="552"/>
-      <c r="Q2" s="552"/>
-      <c r="R2" s="552"/>
-      <c r="S2" s="552"/>
-      <c r="T2" s="552"/>
-      <c r="U2" s="552"/>
+      <c r="D2" s="555"/>
+      <c r="E2" s="555"/>
+      <c r="F2" s="555"/>
+      <c r="G2" s="555"/>
+      <c r="H2" s="555"/>
+      <c r="I2" s="555"/>
+      <c r="J2" s="555"/>
+      <c r="K2" s="555"/>
+      <c r="L2" s="555"/>
+      <c r="M2" s="555"/>
+      <c r="N2" s="555"/>
+      <c r="O2" s="555"/>
+      <c r="P2" s="555"/>
+      <c r="Q2" s="555"/>
+      <c r="R2" s="555"/>
+      <c r="S2" s="555"/>
+      <c r="T2" s="555"/>
+      <c r="U2" s="555"/>
       <c r="V2" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="W2" s="555">
+      <c r="W2" s="558">
         <v>44698</v>
       </c>
-      <c r="X2" s="556"/>
+      <c r="X2" s="559"/>
     </row>
     <row r="3" spans="1:24" ht="33.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="549"/>
-      <c r="B3" s="550"/>
-      <c r="C3" s="553"/>
-      <c r="D3" s="554"/>
-      <c r="E3" s="554"/>
-      <c r="F3" s="554"/>
-      <c r="G3" s="554"/>
-      <c r="H3" s="554"/>
-      <c r="I3" s="554"/>
-      <c r="J3" s="554"/>
-      <c r="K3" s="554"/>
-      <c r="L3" s="554"/>
-      <c r="M3" s="554"/>
-      <c r="N3" s="554"/>
-      <c r="O3" s="554"/>
-      <c r="P3" s="554"/>
-      <c r="Q3" s="554"/>
-      <c r="R3" s="554"/>
-      <c r="S3" s="554"/>
-      <c r="T3" s="554"/>
-      <c r="U3" s="554"/>
+      <c r="A3" s="552"/>
+      <c r="B3" s="553"/>
+      <c r="C3" s="556"/>
+      <c r="D3" s="557"/>
+      <c r="E3" s="557"/>
+      <c r="F3" s="557"/>
+      <c r="G3" s="557"/>
+      <c r="H3" s="557"/>
+      <c r="I3" s="557"/>
+      <c r="J3" s="557"/>
+      <c r="K3" s="557"/>
+      <c r="L3" s="557"/>
+      <c r="M3" s="557"/>
+      <c r="N3" s="557"/>
+      <c r="O3" s="557"/>
+      <c r="P3" s="557"/>
+      <c r="Q3" s="557"/>
+      <c r="R3" s="557"/>
+      <c r="S3" s="557"/>
+      <c r="T3" s="557"/>
+      <c r="U3" s="557"/>
       <c r="V3" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="W3" s="557">
+      <c r="W3" s="560">
         <v>44698</v>
       </c>
-      <c r="X3" s="558"/>
+      <c r="X3" s="561"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
@@ -16833,26 +17371,26 @@
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
-      <c r="D5" s="566"/>
-      <c r="E5" s="567"/>
-      <c r="F5" s="567"/>
-      <c r="G5" s="567"/>
-      <c r="H5" s="567"/>
-      <c r="I5" s="567"/>
-      <c r="J5" s="567"/>
-      <c r="K5" s="567"/>
-      <c r="L5" s="567"/>
-      <c r="M5" s="567"/>
-      <c r="N5" s="567"/>
-      <c r="O5" s="567"/>
-      <c r="P5" s="567"/>
-      <c r="Q5" s="567"/>
-      <c r="R5" s="567"/>
-      <c r="S5" s="567"/>
-      <c r="T5" s="567"/>
-      <c r="U5" s="567"/>
-      <c r="V5" s="567"/>
-      <c r="W5" s="568"/>
+      <c r="D5" s="569"/>
+      <c r="E5" s="570"/>
+      <c r="F5" s="570"/>
+      <c r="G5" s="570"/>
+      <c r="H5" s="570"/>
+      <c r="I5" s="570"/>
+      <c r="J5" s="570"/>
+      <c r="K5" s="570"/>
+      <c r="L5" s="570"/>
+      <c r="M5" s="570"/>
+      <c r="N5" s="570"/>
+      <c r="O5" s="570"/>
+      <c r="P5" s="570"/>
+      <c r="Q5" s="570"/>
+      <c r="R5" s="570"/>
+      <c r="S5" s="570"/>
+      <c r="T5" s="570"/>
+      <c r="U5" s="570"/>
+      <c r="V5" s="570"/>
+      <c r="W5" s="571"/>
       <c r="X5" s="14"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -16861,104 +17399,104 @@
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
-      <c r="D6" s="569"/>
-      <c r="E6" s="570"/>
-      <c r="F6" s="570"/>
-      <c r="G6" s="570"/>
-      <c r="H6" s="570"/>
-      <c r="I6" s="570"/>
-      <c r="J6" s="570"/>
-      <c r="K6" s="570"/>
-      <c r="L6" s="570"/>
-      <c r="M6" s="570"/>
-      <c r="N6" s="570"/>
-      <c r="O6" s="570"/>
-      <c r="P6" s="570"/>
-      <c r="Q6" s="570"/>
-      <c r="R6" s="570"/>
-      <c r="S6" s="570"/>
-      <c r="T6" s="570"/>
-      <c r="U6" s="570"/>
-      <c r="V6" s="570"/>
-      <c r="W6" s="571"/>
+      <c r="D6" s="572"/>
+      <c r="E6" s="573"/>
+      <c r="F6" s="573"/>
+      <c r="G6" s="573"/>
+      <c r="H6" s="573"/>
+      <c r="I6" s="573"/>
+      <c r="J6" s="573"/>
+      <c r="K6" s="573"/>
+      <c r="L6" s="573"/>
+      <c r="M6" s="573"/>
+      <c r="N6" s="573"/>
+      <c r="O6" s="573"/>
+      <c r="P6" s="573"/>
+      <c r="Q6" s="573"/>
+      <c r="R6" s="573"/>
+      <c r="S6" s="573"/>
+      <c r="T6" s="573"/>
+      <c r="U6" s="573"/>
+      <c r="V6" s="573"/>
+      <c r="W6" s="574"/>
       <c r="X6" s="14"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
-      <c r="D7" s="569"/>
-      <c r="E7" s="570"/>
-      <c r="F7" s="570"/>
-      <c r="G7" s="570"/>
-      <c r="H7" s="570"/>
-      <c r="I7" s="570"/>
-      <c r="J7" s="570"/>
-      <c r="K7" s="570"/>
-      <c r="L7" s="570"/>
-      <c r="M7" s="570"/>
-      <c r="N7" s="570"/>
-      <c r="O7" s="570"/>
-      <c r="P7" s="570"/>
-      <c r="Q7" s="570"/>
-      <c r="R7" s="570"/>
-      <c r="S7" s="570"/>
-      <c r="T7" s="570"/>
-      <c r="U7" s="570"/>
-      <c r="V7" s="570"/>
-      <c r="W7" s="571"/>
+      <c r="D7" s="572"/>
+      <c r="E7" s="573"/>
+      <c r="F7" s="573"/>
+      <c r="G7" s="573"/>
+      <c r="H7" s="573"/>
+      <c r="I7" s="573"/>
+      <c r="J7" s="573"/>
+      <c r="K7" s="573"/>
+      <c r="L7" s="573"/>
+      <c r="M7" s="573"/>
+      <c r="N7" s="573"/>
+      <c r="O7" s="573"/>
+      <c r="P7" s="573"/>
+      <c r="Q7" s="573"/>
+      <c r="R7" s="573"/>
+      <c r="S7" s="573"/>
+      <c r="T7" s="573"/>
+      <c r="U7" s="573"/>
+      <c r="V7" s="573"/>
+      <c r="W7" s="574"/>
       <c r="X7" s="14"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
-      <c r="D8" s="569"/>
-      <c r="E8" s="570"/>
-      <c r="F8" s="570"/>
-      <c r="G8" s="570"/>
-      <c r="H8" s="570"/>
-      <c r="I8" s="570"/>
-      <c r="J8" s="570"/>
-      <c r="K8" s="570"/>
-      <c r="L8" s="570"/>
-      <c r="M8" s="570"/>
-      <c r="N8" s="570"/>
-      <c r="O8" s="570"/>
-      <c r="P8" s="570"/>
-      <c r="Q8" s="570"/>
-      <c r="R8" s="570"/>
-      <c r="S8" s="570"/>
-      <c r="T8" s="570"/>
-      <c r="U8" s="570"/>
-      <c r="V8" s="570"/>
-      <c r="W8" s="571"/>
+      <c r="D8" s="572"/>
+      <c r="E8" s="573"/>
+      <c r="F8" s="573"/>
+      <c r="G8" s="573"/>
+      <c r="H8" s="573"/>
+      <c r="I8" s="573"/>
+      <c r="J8" s="573"/>
+      <c r="K8" s="573"/>
+      <c r="L8" s="573"/>
+      <c r="M8" s="573"/>
+      <c r="N8" s="573"/>
+      <c r="O8" s="573"/>
+      <c r="P8" s="573"/>
+      <c r="Q8" s="573"/>
+      <c r="R8" s="573"/>
+      <c r="S8" s="573"/>
+      <c r="T8" s="573"/>
+      <c r="U8" s="573"/>
+      <c r="V8" s="573"/>
+      <c r="W8" s="574"/>
       <c r="X8" s="14"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="572"/>
-      <c r="E9" s="573"/>
-      <c r="F9" s="573"/>
-      <c r="G9" s="573"/>
-      <c r="H9" s="573"/>
-      <c r="I9" s="573"/>
-      <c r="J9" s="573"/>
-      <c r="K9" s="573"/>
-      <c r="L9" s="573"/>
-      <c r="M9" s="573"/>
-      <c r="N9" s="573"/>
-      <c r="O9" s="573"/>
-      <c r="P9" s="573"/>
-      <c r="Q9" s="573"/>
-      <c r="R9" s="573"/>
-      <c r="S9" s="573"/>
-      <c r="T9" s="573"/>
-      <c r="U9" s="573"/>
-      <c r="V9" s="573"/>
-      <c r="W9" s="574"/>
+      <c r="D9" s="575"/>
+      <c r="E9" s="576"/>
+      <c r="F9" s="576"/>
+      <c r="G9" s="576"/>
+      <c r="H9" s="576"/>
+      <c r="I9" s="576"/>
+      <c r="J9" s="576"/>
+      <c r="K9" s="576"/>
+      <c r="L9" s="576"/>
+      <c r="M9" s="576"/>
+      <c r="N9" s="576"/>
+      <c r="O9" s="576"/>
+      <c r="P9" s="576"/>
+      <c r="Q9" s="576"/>
+      <c r="R9" s="576"/>
+      <c r="S9" s="576"/>
+      <c r="T9" s="576"/>
+      <c r="U9" s="576"/>
+      <c r="V9" s="576"/>
+      <c r="W9" s="577"/>
       <c r="X9" s="14"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
@@ -16988,58 +17526,58 @@
       <c r="X10" s="14"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="559" t="s">
+      <c r="A11" s="562" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="560"/>
-      <c r="C11" s="560"/>
-      <c r="D11" s="560"/>
-      <c r="E11" s="560"/>
-      <c r="F11" s="560"/>
-      <c r="G11" s="560"/>
-      <c r="H11" s="560"/>
-      <c r="I11" s="560"/>
-      <c r="J11" s="560"/>
-      <c r="K11" s="560"/>
-      <c r="L11" s="560"/>
-      <c r="M11" s="560"/>
-      <c r="N11" s="560"/>
-      <c r="O11" s="560"/>
-      <c r="P11" s="560"/>
-      <c r="Q11" s="560"/>
-      <c r="R11" s="560"/>
-      <c r="S11" s="560"/>
-      <c r="T11" s="560"/>
-      <c r="U11" s="560"/>
-      <c r="V11" s="560"/>
-      <c r="W11" s="560"/>
-      <c r="X11" s="561"/>
+      <c r="B11" s="563"/>
+      <c r="C11" s="563"/>
+      <c r="D11" s="563"/>
+      <c r="E11" s="563"/>
+      <c r="F11" s="563"/>
+      <c r="G11" s="563"/>
+      <c r="H11" s="563"/>
+      <c r="I11" s="563"/>
+      <c r="J11" s="563"/>
+      <c r="K11" s="563"/>
+      <c r="L11" s="563"/>
+      <c r="M11" s="563"/>
+      <c r="N11" s="563"/>
+      <c r="O11" s="563"/>
+      <c r="P11" s="563"/>
+      <c r="Q11" s="563"/>
+      <c r="R11" s="563"/>
+      <c r="S11" s="563"/>
+      <c r="T11" s="563"/>
+      <c r="U11" s="563"/>
+      <c r="V11" s="563"/>
+      <c r="W11" s="563"/>
+      <c r="X11" s="564"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12" s="562"/>
-      <c r="B12" s="563"/>
-      <c r="C12" s="563"/>
-      <c r="D12" s="563"/>
-      <c r="E12" s="563"/>
-      <c r="F12" s="563"/>
-      <c r="G12" s="563"/>
-      <c r="H12" s="563"/>
-      <c r="I12" s="564"/>
-      <c r="J12" s="563"/>
-      <c r="K12" s="563"/>
-      <c r="L12" s="563"/>
-      <c r="M12" s="563"/>
-      <c r="N12" s="563"/>
-      <c r="O12" s="563"/>
-      <c r="P12" s="563"/>
-      <c r="Q12" s="563"/>
-      <c r="R12" s="563"/>
-      <c r="S12" s="563"/>
-      <c r="T12" s="563"/>
-      <c r="U12" s="563"/>
-      <c r="V12" s="563"/>
-      <c r="W12" s="563"/>
-      <c r="X12" s="565"/>
+      <c r="A12" s="565"/>
+      <c r="B12" s="566"/>
+      <c r="C12" s="566"/>
+      <c r="D12" s="566"/>
+      <c r="E12" s="566"/>
+      <c r="F12" s="566"/>
+      <c r="G12" s="566"/>
+      <c r="H12" s="566"/>
+      <c r="I12" s="567"/>
+      <c r="J12" s="566"/>
+      <c r="K12" s="566"/>
+      <c r="L12" s="566"/>
+      <c r="M12" s="566"/>
+      <c r="N12" s="566"/>
+      <c r="O12" s="566"/>
+      <c r="P12" s="566"/>
+      <c r="Q12" s="566"/>
+      <c r="R12" s="566"/>
+      <c r="S12" s="566"/>
+      <c r="T12" s="566"/>
+      <c r="U12" s="566"/>
+      <c r="V12" s="566"/>
+      <c r="W12" s="566"/>
+      <c r="X12" s="568"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="29"/>
@@ -18849,11 +19387,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q94"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -18863,54 +19401,54 @@
   <sheetData>
     <row r="1" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:17" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="547" t="s">
+      <c r="A2" s="550" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="548"/>
-      <c r="C2" s="551" t="s">
+      <c r="B2" s="551"/>
+      <c r="C2" s="554" t="s">
         <v>119</v>
       </c>
-      <c r="D2" s="552"/>
-      <c r="E2" s="552"/>
-      <c r="F2" s="552"/>
-      <c r="G2" s="552"/>
-      <c r="H2" s="552"/>
-      <c r="I2" s="552"/>
-      <c r="J2" s="552"/>
-      <c r="K2" s="552"/>
-      <c r="L2" s="552"/>
-      <c r="M2" s="552"/>
-      <c r="N2" s="552"/>
+      <c r="D2" s="555"/>
+      <c r="E2" s="555"/>
+      <c r="F2" s="555"/>
+      <c r="G2" s="555"/>
+      <c r="H2" s="555"/>
+      <c r="I2" s="555"/>
+      <c r="J2" s="555"/>
+      <c r="K2" s="555"/>
+      <c r="L2" s="555"/>
+      <c r="M2" s="555"/>
+      <c r="N2" s="555"/>
       <c r="O2" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="P2" s="555">
+      <c r="P2" s="558">
         <v>44698</v>
       </c>
-      <c r="Q2" s="556"/>
+      <c r="Q2" s="559"/>
     </row>
     <row r="3" spans="1:17" ht="33.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="549"/>
-      <c r="B3" s="550"/>
-      <c r="C3" s="553"/>
-      <c r="D3" s="554"/>
-      <c r="E3" s="554"/>
-      <c r="F3" s="554"/>
-      <c r="G3" s="554"/>
-      <c r="H3" s="554"/>
-      <c r="I3" s="554"/>
-      <c r="J3" s="554"/>
-      <c r="K3" s="554"/>
-      <c r="L3" s="554"/>
-      <c r="M3" s="554"/>
-      <c r="N3" s="554"/>
+      <c r="A3" s="552"/>
+      <c r="B3" s="553"/>
+      <c r="C3" s="556"/>
+      <c r="D3" s="557"/>
+      <c r="E3" s="557"/>
+      <c r="F3" s="557"/>
+      <c r="G3" s="557"/>
+      <c r="H3" s="557"/>
+      <c r="I3" s="557"/>
+      <c r="J3" s="557"/>
+      <c r="K3" s="557"/>
+      <c r="L3" s="557"/>
+      <c r="M3" s="557"/>
+      <c r="N3" s="557"/>
       <c r="O3" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="557">
+      <c r="P3" s="560">
         <v>44698</v>
       </c>
-      <c r="Q3" s="558"/>
+      <c r="Q3" s="561"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
@@ -18932,7 +19470,7 @@
       <c r="Q4" s="14"/>
     </row>
     <row r="5" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A5" s="576" t="s">
+      <c r="A5" s="540" t="s">
         <v>121</v>
       </c>
       <c r="B5" s="73"/>
@@ -18958,25 +19496,25 @@
       </c>
       <c r="B6" s="18"/>
       <c r="C6" s="31"/>
-      <c r="D6" s="577" t="s">
+      <c r="D6" s="541" t="s">
         <v>125</v>
       </c>
       <c r="E6" s="18"/>
-      <c r="F6" s="575" t="s">
+      <c r="F6" s="539" t="s">
         <v>29</v>
       </c>
       <c r="G6" s="18"/>
       <c r="H6" s="31"/>
-      <c r="I6" s="577" t="s">
+      <c r="I6" s="541" t="s">
         <v>210</v>
       </c>
       <c r="K6" s="18"/>
-      <c r="L6" s="575" t="s">
+      <c r="L6" s="539" t="s">
         <v>29</v>
       </c>
       <c r="M6" s="18"/>
       <c r="N6" s="31"/>
-      <c r="O6" s="577" t="s">
+      <c r="O6" s="541" t="s">
         <v>222</v>
       </c>
       <c r="P6" s="18"/>
@@ -19325,31 +19863,31 @@
       <c r="Q24" s="14"/>
     </row>
     <row r="25" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A25" s="575" t="s">
+      <c r="A25" s="539" t="s">
         <v>29</v>
       </c>
       <c r="B25" s="18"/>
       <c r="C25" s="31"/>
-      <c r="D25" s="577" t="s">
+      <c r="D25" s="541" t="s">
         <v>211</v>
       </c>
       <c r="E25" s="6"/>
-      <c r="F25" s="575" t="s">
+      <c r="F25" s="539" t="s">
         <v>29</v>
       </c>
       <c r="G25" s="18"/>
       <c r="H25" s="31"/>
-      <c r="I25" s="577" t="s">
+      <c r="I25" s="541" t="s">
         <v>372</v>
       </c>
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
-      <c r="L25" s="575" t="s">
+      <c r="L25" s="539" t="s">
         <v>29</v>
       </c>
       <c r="M25" s="18"/>
       <c r="N25" s="31"/>
-      <c r="O25" s="577" t="s">
+      <c r="O25" s="541" t="s">
         <v>212</v>
       </c>
       <c r="P25" s="6"/>
@@ -19755,31 +20293,31 @@
       <c r="Q46" s="14"/>
     </row>
     <row r="47" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A47" s="575" t="s">
+      <c r="A47" s="539" t="s">
         <v>29</v>
       </c>
       <c r="B47" s="18"/>
       <c r="C47" s="31"/>
-      <c r="D47" s="577" t="s">
+      <c r="D47" s="541" t="s">
         <v>213</v>
       </c>
       <c r="E47" s="6"/>
-      <c r="F47" s="575" t="s">
+      <c r="F47" s="539" t="s">
         <v>29</v>
       </c>
       <c r="G47" s="18"/>
       <c r="H47" s="31"/>
-      <c r="I47" s="577" t="s">
+      <c r="I47" s="541" t="s">
         <v>79</v>
       </c>
       <c r="J47" s="6"/>
       <c r="K47" s="6"/>
-      <c r="L47" s="575" t="s">
+      <c r="L47" s="539" t="s">
         <v>29</v>
       </c>
       <c r="M47" s="18"/>
       <c r="N47" s="31"/>
-      <c r="O47" s="577" t="s">
+      <c r="O47" s="541" t="s">
         <v>214</v>
       </c>
       <c r="P47" s="6"/>
@@ -20261,54 +20799,54 @@
       <c r="Q72" s="17"/>
     </row>
     <row r="74" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A74" s="575" t="s">
+      <c r="A74" s="539" t="s">
         <v>29</v>
       </c>
       <c r="B74" s="18"/>
       <c r="C74" s="31"/>
-      <c r="D74" s="577" t="s">
+      <c r="D74" s="541" t="s">
         <v>215</v>
       </c>
-      <c r="F74" s="575" t="s">
+      <c r="F74" s="539" t="s">
         <v>29</v>
       </c>
       <c r="G74" s="18"/>
       <c r="H74" s="31"/>
-      <c r="I74" s="577" t="s">
+      <c r="I74" s="541" t="s">
         <v>370</v>
       </c>
-      <c r="L74" s="575" t="s">
+      <c r="L74" s="539" t="s">
         <v>29</v>
       </c>
       <c r="M74" s="18"/>
       <c r="N74" s="31"/>
-      <c r="O74" s="577" t="s">
+      <c r="O74" s="541" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="94" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A94" s="575" t="s">
+      <c r="A94" s="539" t="s">
         <v>29</v>
       </c>
       <c r="B94" s="18"/>
       <c r="C94" s="31"/>
-      <c r="D94" s="577" t="s">
+      <c r="D94" s="541" t="s">
         <v>354</v>
       </c>
-      <c r="F94" s="575" t="s">
+      <c r="F94" s="539" t="s">
         <v>29</v>
       </c>
       <c r="G94" s="18"/>
       <c r="H94" s="31"/>
-      <c r="I94" s="577" t="s">
+      <c r="I94" s="541" t="s">
         <v>355</v>
       </c>
-      <c r="L94" s="575" t="s">
+      <c r="L94" s="539" t="s">
         <v>29</v>
       </c>
       <c r="M94" s="18"/>
       <c r="N94" s="31"/>
-      <c r="O94" s="577" t="s">
+      <c r="O94" s="541" t="s">
         <v>373</v>
       </c>
     </row>
@@ -20328,11 +20866,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O348"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -20347,50 +20885,50 @@
   <sheetData>
     <row r="1" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:15" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="547" t="s">
+      <c r="A2" s="550" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="548"/>
-      <c r="C2" s="551" t="s">
+      <c r="B2" s="551"/>
+      <c r="C2" s="554" t="s">
         <v>119</v>
       </c>
-      <c r="D2" s="552"/>
-      <c r="E2" s="552"/>
-      <c r="F2" s="552"/>
-      <c r="G2" s="552"/>
-      <c r="H2" s="552"/>
-      <c r="I2" s="552"/>
-      <c r="J2" s="552"/>
-      <c r="K2" s="552"/>
-      <c r="L2" s="552"/>
+      <c r="D2" s="555"/>
+      <c r="E2" s="555"/>
+      <c r="F2" s="555"/>
+      <c r="G2" s="555"/>
+      <c r="H2" s="555"/>
+      <c r="I2" s="555"/>
+      <c r="J2" s="555"/>
+      <c r="K2" s="555"/>
+      <c r="L2" s="555"/>
       <c r="M2" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="555">
+      <c r="N2" s="558">
         <v>44698</v>
       </c>
-      <c r="O2" s="556"/>
+      <c r="O2" s="559"/>
     </row>
     <row r="3" spans="1:15" ht="33.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="549"/>
-      <c r="B3" s="550"/>
-      <c r="C3" s="553"/>
-      <c r="D3" s="554"/>
-      <c r="E3" s="554"/>
-      <c r="F3" s="554"/>
-      <c r="G3" s="554"/>
-      <c r="H3" s="554"/>
-      <c r="I3" s="554"/>
-      <c r="J3" s="554"/>
-      <c r="K3" s="554"/>
-      <c r="L3" s="554"/>
+      <c r="A3" s="552"/>
+      <c r="B3" s="553"/>
+      <c r="C3" s="556"/>
+      <c r="D3" s="557"/>
+      <c r="E3" s="557"/>
+      <c r="F3" s="557"/>
+      <c r="G3" s="557"/>
+      <c r="H3" s="557"/>
+      <c r="I3" s="557"/>
+      <c r="J3" s="557"/>
+      <c r="K3" s="557"/>
+      <c r="L3" s="557"/>
       <c r="M3" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="N3" s="557">
+      <c r="N3" s="560">
         <v>44702</v>
       </c>
-      <c r="O3" s="558"/>
+      <c r="O3" s="561"/>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13"/>

</xml_diff>